<commit_message>
wages and employment update
</commit_message>
<xml_diff>
--- a/data/historical/source/gov_employment_historical.xlsx
+++ b/data/historical/source/gov_employment_historical.xlsx
@@ -178,7 +178,7 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>Government Employment; Year/Year: January 1990 -- November 2015</t>
+    <t>Government Employment; Year/Year: January 1990 -- December 2015</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1091,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1101,6 +1101,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="241">
     <cellStyle name="active" xfId="3"/>
@@ -1645,64 +1646,64 @@
   <dimension ref="A1:BA590"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M304" sqref="M304"/>
+      <pane ySplit="5" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ298" sqref="AJ298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6" style="6" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="12.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5" style="9" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="6.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5" style="9" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9" style="9" bestFit="1" customWidth="1"/>
     <col min="54" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -1721,6 +1722,60 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
+      <c r="AW4" s="6"/>
+      <c r="AX4" s="6"/>
+      <c r="AY4" s="6"/>
+      <c r="AZ4" s="6"/>
+      <c r="BA4" s="6"/>
+    </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
@@ -49702,7 +49757,7 @@
         <v>42278</v>
       </c>
       <c r="B303" s="8">
-        <v>0.40213864643787411</v>
+        <v>0.40670840378375911</v>
       </c>
       <c r="C303" s="8">
         <v>0.26336581511719775</v>
@@ -49863,55 +49918,55 @@
         <v>42309</v>
       </c>
       <c r="B304" s="8">
-        <v>0.42481271697423723</v>
+        <v>0.42024483829709486</v>
       </c>
       <c r="C304" s="8">
-        <v>0.36861506055818249</v>
+        <v>-7.8988941548186239E-2</v>
       </c>
       <c r="D304" s="8">
         <v>-2.3170731707317143</v>
       </c>
       <c r="E304" s="8">
-        <v>0.48673643222195184</v>
+        <v>0.41372596738867018</v>
       </c>
       <c r="F304" s="8">
         <v>-0.18770530267480323</v>
       </c>
       <c r="G304" s="8">
-        <v>1.5908250092489937</v>
+        <v>1.2660829530973889</v>
       </c>
       <c r="H304" s="8">
-        <v>0.97727827999022721</v>
+        <v>1.0750061079892443</v>
       </c>
       <c r="I304" s="8">
         <v>4.2122999157537623E-2</v>
       </c>
       <c r="J304" s="8">
-        <v>1.2269938650306704</v>
+        <v>1.073619631901845</v>
       </c>
       <c r="K304" s="8">
-        <v>-0.25412960609910812</v>
+        <v>-0.16941973739940946</v>
       </c>
       <c r="L304" s="8">
-        <v>-0.49146884272998714</v>
+        <v>-0.5378338278931919</v>
       </c>
       <c r="M304" s="8">
-        <v>1.0167029774872911</v>
+        <v>1.0893246187363834</v>
       </c>
       <c r="N304" s="8">
-        <v>0.32154340836012174</v>
+        <v>0.16077170418005515</v>
       </c>
       <c r="O304" s="8">
-        <v>8.3056478405310885E-2</v>
+        <v>0</v>
       </c>
       <c r="P304" s="8">
-        <v>-6.0139523694972344E-2</v>
+        <v>-8.4195333172953066E-2</v>
       </c>
       <c r="Q304" s="8">
-        <v>1.1464670098268681</v>
+        <v>1.4740290126345372</v>
       </c>
       <c r="R304" s="8">
-        <v>-0.34870205346766137</v>
+        <v>-0.27121270825263288</v>
       </c>
       <c r="S304" s="8">
         <v>-1.1627906976744187</v>
@@ -49923,31 +49978,31 @@
         <v>-1.8343014368694586</v>
       </c>
       <c r="V304" s="8">
-        <v>0</v>
+        <v>-0.20000000000000281</v>
       </c>
       <c r="W304" s="8">
-        <v>1.4006707437364418</v>
+        <v>1.3414874728743478</v>
       </c>
       <c r="X304" s="8">
-        <v>1.469620530818172</v>
+        <v>1.4257512612415004</v>
       </c>
       <c r="Y304" s="8">
-        <v>-1.2613521695257317</v>
+        <v>-1.3286242852337669</v>
       </c>
       <c r="Z304" s="8">
-        <v>-0.80817684811028712</v>
+        <v>-0.73686712621819972</v>
       </c>
       <c r="AA304" s="8">
-        <v>0.36659877800407564</v>
+        <v>0.52953156822811054</v>
       </c>
       <c r="AB304" s="8">
-        <v>0.16199953714417695</v>
+        <v>0.1388567461235746</v>
       </c>
       <c r="AC304" s="8">
         <v>0.22753128555175042</v>
       </c>
       <c r="AD304" s="8">
-        <v>0.93240093240092914</v>
+        <v>0.75757575757576423</v>
       </c>
       <c r="AE304" s="8">
         <v>1.7681728880157284</v>
@@ -49959,112 +50014,270 @@
         <v>-3.2123353678131301E-2</v>
       </c>
       <c r="AH304" s="8">
-        <v>0.15641293013554897</v>
+        <v>0.10427528675703264</v>
       </c>
       <c r="AI304" s="8">
-        <v>-0.22216051096917835</v>
+        <v>-0.23604554290475496</v>
       </c>
       <c r="AJ304" s="8">
-        <v>0.37804536544384371</v>
+        <v>0.35004200504060484</v>
       </c>
       <c r="AK304" s="8">
         <v>0.37267080745341263</v>
       </c>
       <c r="AL304" s="8">
-        <v>0.64831966128606655</v>
+        <v>0.62185763429479302</v>
       </c>
       <c r="AM304" s="8">
         <v>0.25854639471415608</v>
       </c>
       <c r="AN304" s="8">
-        <v>2.4915824915824838</v>
+        <v>2.2558922558922521</v>
       </c>
       <c r="AO304" s="8">
-        <v>-0.47948103229445455</v>
+        <v>-0.53589056550558001</v>
       </c>
       <c r="AP304" s="8">
-        <v>-1.0000000000000024</v>
+        <v>-1.1666666666666714</v>
       </c>
       <c r="AQ304" s="8">
-        <v>1.0022271714922113</v>
+        <v>0.94654788418709201</v>
       </c>
       <c r="AR304" s="8">
-        <v>0.63938618925831203</v>
+        <v>0.51150895140663877</v>
       </c>
       <c r="AS304" s="8">
-        <v>-0.18774935461159617</v>
+        <v>0.23468669326449187</v>
       </c>
       <c r="AT304" s="8">
-        <v>1.4049991831400073</v>
+        <v>1.4649022490878447</v>
       </c>
       <c r="AU304" s="8">
-        <v>2.0417028670721189</v>
+        <v>1.9548218940052129</v>
       </c>
       <c r="AV304" s="8">
         <v>2.1505376344086073</v>
       </c>
       <c r="AW304" s="8">
-        <v>0.11309018942607693</v>
+        <v>1.4136273678261625E-2</v>
       </c>
       <c r="AX304" s="8">
-        <v>1.605049594229031</v>
+        <v>1.7673579801623003</v>
       </c>
       <c r="AY304" s="8">
-        <v>-1.0403120936281032</v>
+        <v>-1.1703511053316069</v>
       </c>
       <c r="AZ304" s="8">
-        <v>-0.84398360260429217</v>
+        <v>-0.89221123703882055</v>
       </c>
       <c r="BA304" s="8">
-        <v>1.2587412587412667</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A305" s="7"/>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+        <v>0.97902097902098295</v>
+      </c>
+    </row>
+    <row r="305" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A305" s="7">
+        <v>42339</v>
+      </c>
+      <c r="B305" s="9">
+        <v>0.45201351474751161</v>
+      </c>
+      <c r="C305" s="9">
+        <v>0</v>
+      </c>
+      <c r="D305" s="9">
+        <v>-2.0731707317073207</v>
+      </c>
+      <c r="E305" s="9">
+        <v>-2.4324981756269213E-2</v>
+      </c>
+      <c r="F305" s="9">
+        <v>-0.23452157598499063</v>
+      </c>
+      <c r="G305" s="9">
+        <v>1.4598840317473374</v>
+      </c>
+      <c r="H305" s="9">
+        <v>1.2955267660718539</v>
+      </c>
+      <c r="I305" s="9">
+        <v>-0.16827934371054998</v>
+      </c>
+      <c r="J305" s="9">
+        <v>0.91883614088822141</v>
+      </c>
+      <c r="K305" s="9">
+        <v>0.16927634363096794</v>
+      </c>
+      <c r="L305" s="9">
+        <v>-0.53738534235151991</v>
+      </c>
+      <c r="M305" s="9">
+        <v>0.84363636363635697</v>
+      </c>
+      <c r="N305" s="9">
+        <v>0.48076923076923767</v>
+      </c>
+      <c r="O305" s="9">
+        <v>0.83194675540765384</v>
+      </c>
+      <c r="P305" s="9">
+        <v>-2.4061597690092092E-2</v>
+      </c>
+      <c r="Q305" s="9">
+        <v>1.5377446411929225</v>
+      </c>
+      <c r="R305" s="9">
+        <v>-0.54326736515327023</v>
+      </c>
+      <c r="S305" s="9">
+        <v>-0.9701202949165697</v>
+      </c>
+      <c r="T305" s="9">
+        <v>0.40049291435611656</v>
+      </c>
+      <c r="U305" s="9">
+        <v>-1.8343014368694586</v>
+      </c>
+      <c r="V305" s="9">
+        <v>0</v>
+      </c>
+      <c r="W305" s="9">
+        <v>1.3617525162818305</v>
+      </c>
+      <c r="X305" s="9">
+        <v>1.4892685063512821</v>
+      </c>
+      <c r="Y305" s="9">
+        <v>-1.2264784946236673</v>
+      </c>
+      <c r="Z305" s="9">
+        <v>0.78834209268990785</v>
+      </c>
+      <c r="AA305" s="9">
+        <v>8.1466395112011661E-2</v>
+      </c>
+      <c r="AB305" s="9">
+        <v>0.44032444959443268</v>
+      </c>
+      <c r="AC305" s="9">
+        <v>0.79908675799087081</v>
+      </c>
+      <c r="AD305" s="9">
+        <v>1.048340128130467</v>
+      </c>
+      <c r="AE305" s="9">
+        <v>2.2950819672131146</v>
+      </c>
+      <c r="AF305" s="9">
+        <v>-2.7685492801771874</v>
+      </c>
+      <c r="AG305" s="9">
+        <v>0.11244979919679446</v>
+      </c>
+      <c r="AH305" s="9">
+        <v>0.36534446764092748</v>
+      </c>
+      <c r="AI305" s="9">
+        <v>-0.21538247759326817</v>
+      </c>
+      <c r="AJ305" s="9">
+        <v>0.1816149762503588</v>
+      </c>
+      <c r="AK305" s="9">
+        <v>-0.12406947890818154</v>
+      </c>
+      <c r="AL305" s="9">
+        <v>9.2214464497422183E-2</v>
+      </c>
+      <c r="AM305" s="9">
+        <v>0.20114942528735308</v>
+      </c>
+      <c r="AN305" s="9">
+        <v>2.2498321020819301</v>
+      </c>
+      <c r="AO305" s="9">
+        <v>-0.26821005081874327</v>
+      </c>
+      <c r="AP305" s="9">
+        <v>-1.3311148086522535</v>
+      </c>
+      <c r="AQ305" s="9">
+        <v>1.1111111111111112</v>
+      </c>
+      <c r="AR305" s="9">
+        <v>1.025641025641022</v>
+      </c>
+      <c r="AS305" s="9">
+        <v>0.5153431717029856</v>
+      </c>
+      <c r="AT305" s="9">
+        <v>1.3903220550697952</v>
+      </c>
+      <c r="AU305" s="9">
+        <v>1.7818339852238134</v>
+      </c>
+      <c r="AV305" s="9">
+        <v>1.6071428571428545</v>
+      </c>
+      <c r="AW305" s="9">
+        <v>-0.14120304998587968</v>
+      </c>
+      <c r="AX305" s="9">
+        <v>1.5978456014362616</v>
+      </c>
+      <c r="AY305" s="9">
+        <v>-1.1053315994798549</v>
+      </c>
+      <c r="AZ305" s="9">
+        <v>0.50933786078097643</v>
+      </c>
+      <c r="BA305" s="9">
+        <v>1.5427769985974875</v>
+      </c>
+    </row>
+    <row r="306" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A306" s="7"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A307" s="7"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A308" s="7"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A309" s="7"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A310" s="7"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A311" s="7"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A312" s="7"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A313" s="7"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A314" s="7"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A315" s="7"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A316" s="7"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A317" s="7"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A318" s="7"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A319" s="7"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A320" s="7"/>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
earning and emp data
</commit_message>
<xml_diff>
--- a/data/historical/source/gov_employment_historical.xlsx
+++ b/data/historical/source/gov_employment_historical.xlsx
@@ -178,7 +178,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Government Employment; Year/Year: January 1990 -- January 2017</t>
+    <t>Government Employment; Year/Year: January 1990 -- February 2017</t>
   </si>
 </sst>
 </file>
@@ -1647,7 +1647,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B290" sqref="B290"/>
+      <selection pane="bottomLeft" activeCell="B304" sqref="B304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -52178,52 +52178,52 @@
         <v>0.53008216273522391</v>
       </c>
       <c r="D318" s="9">
-        <v>-1.4652014652014684</v>
+        <v>-0.8547008547008581</v>
       </c>
       <c r="E318" s="9">
-        <v>0.14659174199852576</v>
+        <v>0.31761544099682659</v>
       </c>
       <c r="F318" s="9">
         <v>-0.70488721804511278</v>
       </c>
       <c r="G318" s="9">
-        <v>2.4006755669937192</v>
+        <v>2.1272317838185471</v>
       </c>
       <c r="H318" s="9">
-        <v>1.8160377358490538</v>
+        <v>2.1462264150943451</v>
       </c>
       <c r="I318" s="9">
         <v>-1.8479630407391878</v>
       </c>
       <c r="J318" s="9">
-        <v>-0.92024539877301925</v>
+        <v>-0.30674846625767305</v>
       </c>
       <c r="K318" s="9">
         <v>0.50146259924780134</v>
       </c>
       <c r="L318" s="9">
-        <v>1.5924153166421164</v>
+        <v>1.5555964653902672</v>
       </c>
       <c r="M318" s="9">
-        <v>1.65835045494571</v>
+        <v>1.7170531259172359</v>
       </c>
       <c r="N318" s="9">
-        <v>1.2038523274478332</v>
+        <v>1.0433386837881313</v>
       </c>
       <c r="O318" s="9">
-        <v>2.1648626144879337</v>
+        <v>3.330557868442964</v>
       </c>
       <c r="P318" s="9">
-        <v>-0.14478764478763656</v>
+        <v>8.4459459459464953E-2</v>
       </c>
       <c r="Q318" s="9">
-        <v>1.2195121951219621</v>
+        <v>1.0553470919324579</v>
       </c>
       <c r="R318" s="9">
         <v>0.5058365758754908</v>
       </c>
       <c r="S318" s="9">
-        <v>-3.9169604387004599E-2</v>
+        <v>-7.8339208773998054E-2</v>
       </c>
       <c r="T318" s="9">
         <v>-0.18796992481201941</v>
@@ -52235,31 +52235,31 @@
         <v>0.30272452068618705</v>
       </c>
       <c r="W318" s="9">
-        <v>0.47723205408630626</v>
+        <v>1.2925034798170612</v>
       </c>
       <c r="X318" s="9">
         <v>2.1068973164781553</v>
       </c>
       <c r="Y318" s="9">
-        <v>2.6559085560598534</v>
+        <v>2.4541939821818834</v>
       </c>
       <c r="Z318" s="9">
         <v>1.041173686701367</v>
       </c>
       <c r="AA318" s="9">
-        <v>0.65573770491803041</v>
+        <v>0.53278688524590634</v>
       </c>
       <c r="AB318" s="9">
-        <v>0.50878815911194397</v>
+        <v>0.64754856614246337</v>
       </c>
       <c r="AC318" s="9">
         <v>0.9933774834437149</v>
       </c>
       <c r="AD318" s="9">
-        <v>-0.17472335468840008</v>
+        <v>-0.29120559114735006</v>
       </c>
       <c r="AE318" s="9">
-        <v>2.0525978191148098</v>
+        <v>2.3733162283514999</v>
       </c>
       <c r="AF318" s="9">
         <v>0.88593576965669674</v>
@@ -52268,7 +52268,7 @@
         <v>-0.61969993476843899</v>
       </c>
       <c r="AH318" s="9">
-        <v>-1.3061650992685474</v>
+        <v>-0.99268547544409913</v>
       </c>
       <c r="AI318" s="9">
         <v>0.5472809144440659</v>
@@ -52280,31 +52280,31 @@
         <v>1.5643802647412892</v>
       </c>
       <c r="AL318" s="9">
-        <v>-0.42591636551367512</v>
+        <v>-0.27103768714505799</v>
       </c>
       <c r="AM318" s="9">
         <v>0.19790783149561453</v>
       </c>
       <c r="AN318" s="9">
-        <v>1.2179065174456842</v>
+        <v>0.42791310072416433</v>
       </c>
       <c r="AO318" s="9">
-        <v>-9.9686698946175656E-2</v>
+        <v>-0.25633722586158758</v>
       </c>
       <c r="AP318" s="9">
         <v>0.49833887043188896</v>
       </c>
       <c r="AQ318" s="9">
-        <v>0.66280033140015937</v>
+        <v>0.71803369235017001</v>
       </c>
       <c r="AR318" s="9">
-        <v>2.051282051282044</v>
+        <v>2.1794871794871833</v>
       </c>
       <c r="AS318" s="9">
-        <v>0.28202115158636631</v>
+        <v>1.6451233842538191</v>
       </c>
       <c r="AT318" s="9">
-        <v>2.2168522798907362</v>
+        <v>2.1328010086152625</v>
       </c>
       <c r="AU318" s="9">
         <v>1.9982993197278986</v>
@@ -52313,23 +52313,181 @@
         <v>0.36036036036036551</v>
       </c>
       <c r="AW318" s="9">
-        <v>0.37985368598762598</v>
+        <v>0.36578503095104431</v>
       </c>
       <c r="AX318" s="9">
-        <v>1.8005295675198669</v>
+        <v>2.0300088261253313</v>
       </c>
       <c r="AY318" s="9">
         <v>0.71197411003235878</v>
       </c>
       <c r="AZ318" s="9">
-        <v>0.60960741282613995</v>
+        <v>0.7559131919044052</v>
       </c>
       <c r="BA318" s="9">
-        <v>-1.8105849582172664</v>
+        <v>-1.9498607242339716</v>
       </c>
     </row>
     <row r="319" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A319" s="7"/>
+      <c r="A319" s="7">
+        <v>42767</v>
+      </c>
+      <c r="B319" s="9">
+        <v>0.87663804789877997</v>
+      </c>
+      <c r="C319" s="9">
+        <v>0.90209604669674559</v>
+      </c>
+      <c r="D319" s="9">
+        <v>-0.85679314565483811</v>
+      </c>
+      <c r="E319" s="9">
+        <v>0.29275433032448051</v>
+      </c>
+      <c r="F319" s="9">
+        <v>-0.79812206572769417</v>
+      </c>
+      <c r="G319" s="9">
+        <v>1.862107713299608</v>
+      </c>
+      <c r="H319" s="9">
+        <v>1.1997177134791732</v>
+      </c>
+      <c r="I319" s="9">
+        <v>-1.8899622007559851</v>
+      </c>
+      <c r="J319" s="9">
+        <v>-0.92449922958398845</v>
+      </c>
+      <c r="K319" s="9">
+        <v>-0.20885547201336674</v>
+      </c>
+      <c r="L319" s="9">
+        <v>0.8272819192940527</v>
+      </c>
+      <c r="M319" s="9">
+        <v>1.5975377399970823</v>
+      </c>
+      <c r="N319" s="9">
+        <v>0.55599682287528884</v>
+      </c>
+      <c r="O319" s="9">
+        <v>3.4912718204488802</v>
+      </c>
+      <c r="P319" s="9">
+        <v>1.2324794586756804</v>
+      </c>
+      <c r="Q319" s="9">
+        <v>1.4499532273152451</v>
+      </c>
+      <c r="R319" s="9">
+        <v>0.31128404669261145</v>
+      </c>
+      <c r="S319" s="9">
+        <v>-0.66536203522504445</v>
+      </c>
+      <c r="T319" s="9">
+        <v>-0.81530260269675958</v>
+      </c>
+      <c r="U319" s="9">
+        <v>-0.82745939319644157</v>
+      </c>
+      <c r="V319" s="9">
+        <v>0.10030090270811867</v>
+      </c>
+      <c r="W319" s="9">
+        <v>1.9736842105263113</v>
+      </c>
+      <c r="X319" s="9">
+        <v>1.6168327796234796</v>
+      </c>
+      <c r="Y319" s="9">
+        <v>2.3341729638958819</v>
+      </c>
+      <c r="Z319" s="9">
+        <v>0.83115649489432442</v>
+      </c>
+      <c r="AA319" s="9">
+        <v>0.69586573884567682</v>
+      </c>
+      <c r="AB319" s="9">
+        <v>1.3519813519813546</v>
+      </c>
+      <c r="AC319" s="9">
+        <v>1.2141280353200978</v>
+      </c>
+      <c r="AD319" s="9">
+        <v>-0.46592894583575017</v>
+      </c>
+      <c r="AE319" s="9">
+        <v>0.9590792838874681</v>
+      </c>
+      <c r="AF319" s="9">
+        <v>-0.43811610076669388</v>
+      </c>
+      <c r="AG319" s="9">
+        <v>-0.65178425941013518</v>
+      </c>
+      <c r="AH319" s="9">
+        <v>0</v>
+      </c>
+      <c r="AI319" s="9">
+        <v>0.60299417798725019</v>
+      </c>
+      <c r="AJ319" s="9">
+        <v>0.83090984628167841</v>
+      </c>
+      <c r="AK319" s="9">
+        <v>0.9580838323353259</v>
+      </c>
+      <c r="AL319" s="9">
+        <v>-0.59255442483574761</v>
+      </c>
+      <c r="AM319" s="9">
+        <v>0.22611644997173863</v>
+      </c>
+      <c r="AN319" s="9">
+        <v>1.5753199868723373</v>
+      </c>
+      <c r="AO319" s="9">
+        <v>-0.47001851588093829</v>
+      </c>
+      <c r="AP319" s="9">
+        <v>0.33112582781457428</v>
+      </c>
+      <c r="AQ319" s="9">
+        <v>0.55202870549268557</v>
+      </c>
+      <c r="AR319" s="9">
+        <v>2.1766965428937297</v>
+      </c>
+      <c r="AS319" s="9">
+        <v>1.6897441915043392</v>
+      </c>
+      <c r="AT319" s="9">
+        <v>1.7424162905426583</v>
+      </c>
+      <c r="AU319" s="9">
+        <v>2.2495755517826876</v>
+      </c>
+      <c r="AV319" s="9">
+        <v>-0.17985611510791621</v>
+      </c>
+      <c r="AW319" s="9">
+        <v>0.65909409619968184</v>
+      </c>
+      <c r="AX319" s="9">
+        <v>2.2026431718061676</v>
+      </c>
+      <c r="AY319" s="9">
+        <v>0.84251458198313856</v>
+      </c>
+      <c r="AZ319" s="9">
+        <v>1.6341463414634119</v>
+      </c>
+      <c r="BA319" s="9">
+        <v>-1.6736401673640207</v>
+      </c>
     </row>
     <row r="320" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A320" s="7"/>

</xml_diff>

<commit_message>
manual revert of last commit
</commit_message>
<xml_diff>
--- a/data/historical/source/gov_employment_historical.xlsx
+++ b/data/historical/source/gov_employment_historical.xlsx
@@ -183,7 +183,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Government Employment; Year/Year: January 1990 -- September 2017</t>
+    <t>Government Employment; Year/Year: January 1990 -- August 2017</t>
   </si>
 </sst>
 </file>
@@ -1694,8 +1694,8 @@
   <dimension ref="A1:BA590"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A318" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C325" sqref="C325"/>
+      <pane ySplit="5" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AM297" sqref="AM297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -53080,7 +53080,7 @@
         <v>42917</v>
       </c>
       <c r="B324" s="9">
-        <v>0.30552185829177336</v>
+        <v>0.22464842521453926</v>
       </c>
       <c r="C324" s="9">
         <v>-0.36861506055819748</v>
@@ -53241,28 +53241,28 @@
         <v>42948</v>
       </c>
       <c r="B325" s="9">
-        <v>0.17945266935845669</v>
+        <v>3.5890533871691339E-2</v>
       </c>
       <c r="C325" s="9">
-        <v>-0.28810895756941401</v>
+        <v>-0.7595599790466302</v>
       </c>
       <c r="D325" s="9">
-        <v>0.74165636588380013</v>
+        <v>0.61804697156983934</v>
       </c>
       <c r="E325" s="9">
-        <v>1.3882123721383313</v>
+        <v>0.97418412079883099</v>
       </c>
       <c r="F325" s="9">
         <v>-0.61176470588235832</v>
       </c>
       <c r="G325" s="9">
-        <v>1.6565367655821641</v>
+        <v>1.5611965200810283</v>
       </c>
       <c r="H325" s="9">
-        <v>0.86126629422718548</v>
+        <v>0.53538175046553871</v>
       </c>
       <c r="I325" s="9">
-        <v>-1.2303775986423324</v>
+        <v>-1.2728044123886295</v>
       </c>
       <c r="J325" s="9">
         <v>-0.30581039755352118</v>
@@ -53271,13 +53271,13 @@
         <v>-0.37704231252617398</v>
       </c>
       <c r="L325" s="9">
-        <v>0.78167605889837377</v>
+        <v>0.79985457189601472</v>
       </c>
       <c r="M325" s="9">
-        <v>1.4060008696912663</v>
+        <v>2.1887230033338199</v>
       </c>
       <c r="N325" s="9">
-        <v>-2.9687499999999978</v>
+        <v>-3.125</v>
       </c>
       <c r="O325" s="9">
         <v>2.9508196721311428</v>
@@ -53286,16 +53286,16 @@
         <v>-0.37407988415590954</v>
       </c>
       <c r="Q325" s="9">
-        <v>0.27522935779816254</v>
+        <v>1.4220183486238507</v>
       </c>
       <c r="R325" s="9">
-        <v>-7.7279752704786958E-2</v>
+        <v>-0.77279752704791349</v>
       </c>
       <c r="S325" s="9">
-        <v>0.50860719874803717</v>
+        <v>-1.0563380281690098</v>
       </c>
       <c r="T325" s="9">
-        <v>-0.40739580068944259</v>
+        <v>-0.37605766217488101</v>
       </c>
       <c r="U325" s="9">
         <v>-0.7411982705373793</v>
@@ -53304,73 +53304,73 @@
         <v>1.1952191235059646</v>
       </c>
       <c r="W325" s="9">
-        <v>1.1660079051383354</v>
+        <v>1.1264822134387331</v>
       </c>
       <c r="X325" s="9">
         <v>0.48235036176276885</v>
       </c>
       <c r="Y325" s="9">
-        <v>2.5585645456055786</v>
+        <v>2.2761256022595191</v>
       </c>
       <c r="Z325" s="9">
         <v>0.75170307728446994</v>
       </c>
       <c r="AA325" s="9">
-        <v>0.12274959083469024</v>
+        <v>1.0229132569558101</v>
       </c>
       <c r="AB325" s="9">
-        <v>2.4868811316449868</v>
+        <v>1.528633356148754</v>
       </c>
       <c r="AC325" s="9">
         <v>1.2021857923497206</v>
       </c>
       <c r="AD325" s="9">
-        <v>0.2932551319648094</v>
+        <v>5.865102639295855E-2</v>
       </c>
       <c r="AE325" s="9">
-        <v>2.7568922305764447</v>
+        <v>1.8170426065162943</v>
       </c>
       <c r="AF325" s="9">
-        <v>1.3015184381778773</v>
+        <v>0.97613882863339629</v>
       </c>
       <c r="AG325" s="9">
-        <v>-0.66439799060120275</v>
+        <v>-0.69680764867931744</v>
       </c>
       <c r="AH325" s="9">
-        <v>-1.1512297226582882</v>
+        <v>-1.8315018315018317</v>
       </c>
       <c r="AI325" s="9">
-        <v>0.66390041493775309</v>
+        <v>0.65698478561549101</v>
       </c>
       <c r="AJ325" s="9">
         <v>0.83733699382292692</v>
       </c>
       <c r="AK325" s="9">
-        <v>-0.35842293906809691</v>
+        <v>-0.23894862604540359</v>
       </c>
       <c r="AL325" s="9">
-        <v>-0.47435897435898022</v>
+        <v>-0.53846153846154421</v>
       </c>
       <c r="AM325" s="9">
         <v>0</v>
       </c>
       <c r="AN325" s="9">
-        <v>1.2103369316323156</v>
+        <v>1.2757605495584019</v>
       </c>
       <c r="AO325" s="9">
-        <v>-0.71740047826698872</v>
+        <v>-1.3504009002672701</v>
       </c>
       <c r="AP325" s="9">
         <v>-0.98360655737705149</v>
       </c>
       <c r="AQ325" s="9">
-        <v>1.7553483269336194</v>
+        <v>1.5359297860669132</v>
       </c>
       <c r="AR325" s="9">
-        <v>1.7721518987341847</v>
+        <v>1.6455696202531609</v>
       </c>
       <c r="AS325" s="9">
-        <v>1.3333333333333306</v>
+        <v>1.3099415204678415</v>
       </c>
       <c r="AT325" s="9">
         <v>1.4393704048876437</v>
@@ -53385,178 +53385,20 @@
         <v>-0.18156424581004951</v>
       </c>
       <c r="AX325" s="9">
-        <v>2.1939752742469136</v>
+        <v>2.4899878112484886</v>
       </c>
       <c r="AY325" s="9">
         <v>-1.0276172125883074</v>
       </c>
       <c r="AZ325" s="9">
-        <v>-0.50651230101303002</v>
+        <v>-0.26531596719730405</v>
       </c>
       <c r="BA325" s="9">
-        <v>-2.1008403361344534</v>
+        <v>-2.3809523809523845</v>
       </c>
     </row>
     <row r="326" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A326" s="7">
-        <v>42979</v>
-      </c>
-      <c r="B326" s="9">
-        <v>9.4102885821831864E-2</v>
-      </c>
-      <c r="C326" s="9">
-        <v>-0.47393364928910253</v>
-      </c>
-      <c r="D326" s="9">
-        <v>0.86741016109046198</v>
-      </c>
-      <c r="E326" s="9">
-        <v>0.29027576197388621</v>
-      </c>
-      <c r="F326" s="9">
-        <v>-0.47236655644780345</v>
-      </c>
-      <c r="G326" s="9">
-        <v>2.278120550545796</v>
-      </c>
-      <c r="H326" s="9">
-        <v>-6.9848661233995663E-2</v>
-      </c>
-      <c r="I326" s="9">
-        <v>-1.5286624203821633</v>
-      </c>
-      <c r="J326" s="9">
-        <v>-0.15267175572518216</v>
-      </c>
-      <c r="K326" s="9">
-        <v>0.20946795140343527</v>
-      </c>
-      <c r="L326" s="9">
-        <v>0.44384057971015317</v>
-      </c>
-      <c r="M326" s="9">
-        <v>1.1154570476604442</v>
-      </c>
-      <c r="N326" s="9">
-        <v>-0.78864353312302837</v>
-      </c>
-      <c r="O326" s="9">
-        <v>3.6824877250409163</v>
-      </c>
-      <c r="P326" s="9">
-        <v>-0.85244327050066315</v>
-      </c>
-      <c r="Q326" s="9">
-        <v>1.756007393715334</v>
-      </c>
-      <c r="R326" s="9">
-        <v>-0.50193050193050637</v>
-      </c>
-      <c r="S326" s="9">
-        <v>-3.8986354775837326E-2</v>
-      </c>
-      <c r="T326" s="9">
-        <v>-0.56479447756511181</v>
-      </c>
-      <c r="U326" s="9">
-        <v>-1.805385556915555</v>
-      </c>
-      <c r="V326" s="9">
-        <v>0.49850448654037888</v>
-      </c>
-      <c r="W326" s="9">
-        <v>1.6260162601625994</v>
-      </c>
-      <c r="X326" s="9">
-        <v>0.63582547686910262</v>
-      </c>
-      <c r="Y326" s="9">
-        <v>2.0387866732968787</v>
-      </c>
-      <c r="Z326" s="9">
-        <v>1.1748120300751879</v>
-      </c>
-      <c r="AA326" s="9">
-        <v>1.2673753066230558</v>
-      </c>
-      <c r="AB326" s="9">
-        <v>0.54970224461749362</v>
-      </c>
-      <c r="AC326" s="9">
-        <v>1.2008733624454242</v>
-      </c>
-      <c r="AD326" s="9">
-        <v>-0.3454231433506012</v>
-      </c>
-      <c r="AE326" s="9">
-        <v>3.2704402515723201</v>
-      </c>
-      <c r="AF326" s="9">
-        <v>0.55066079295154191</v>
-      </c>
-      <c r="AG326" s="9">
-        <v>-0.43881033642124684</v>
-      </c>
-      <c r="AH326" s="9">
-        <v>-1.6238868517548424</v>
-      </c>
-      <c r="AI326" s="9">
-        <v>0.61417431509213249</v>
-      </c>
-      <c r="AJ326" s="9">
-        <v>1.1059530311305328</v>
-      </c>
-      <c r="AK326" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL326" s="9">
-        <v>-0.39774185270721357</v>
-      </c>
-      <c r="AM326" s="9">
-        <v>0.19796380090497415</v>
-      </c>
-      <c r="AN326" s="9">
-        <v>0.4200323101777097</v>
-      </c>
-      <c r="AO326" s="9">
-        <v>-0.74469579879163528</v>
-      </c>
-      <c r="AP326" s="9">
-        <v>-0.32786885245902103</v>
-      </c>
-      <c r="AQ326" s="9">
-        <v>1.3186813186813218</v>
-      </c>
-      <c r="AR326" s="9">
-        <v>2.405063291139248</v>
-      </c>
-      <c r="AS326" s="9">
-        <v>1.4035087719298245</v>
-      </c>
-      <c r="AT326" s="9">
-        <v>1.3338158506953397</v>
-      </c>
-      <c r="AU326" s="9">
-        <v>1.9991670137442779</v>
-      </c>
-      <c r="AV326" s="9">
-        <v>1.0695187165775426</v>
-      </c>
-      <c r="AW326" s="9">
-        <v>0.14007564084605686</v>
-      </c>
-      <c r="AX326" s="9">
-        <v>2.6406627545737091</v>
-      </c>
-      <c r="AY326" s="9">
-        <v>6.485084306097455E-2</v>
-      </c>
-      <c r="AZ326" s="9">
-        <v>1.4167073766487572</v>
-      </c>
-      <c r="BA326" s="9">
-        <v>-2.2471910112359668</v>
-      </c>
+      <c r="A326" s="7"/>
     </row>
     <row r="327" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A327" s="7"/>

</xml_diff>

<commit_message>
update historical emp and earn
</commit_message>
<xml_diff>
--- a/data/historical/source/gov_employment_historical.xlsx
+++ b/data/historical/source/gov_employment_historical.xlsx
@@ -183,7 +183,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Government Employment; Year/Year: January 1991 -- February 2018</t>
+    <t>Government Employment; Year/Year: January 1991 -- April 2018</t>
   </si>
 </sst>
 </file>
@@ -54207,7 +54207,7 @@
         <v>43132</v>
       </c>
       <c r="B331" s="9">
-        <v>7.1719933659061361E-2</v>
+        <v>5.827244609798736E-2</v>
       </c>
       <c r="C331" s="9">
         <v>0.31241864097890876</v>
@@ -54364,10 +54364,326 @@
       </c>
     </row>
     <row r="332" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A332" s="7"/>
+      <c r="A332" s="7">
+        <v>43160</v>
+      </c>
+      <c r="B332" s="9">
+        <v>3.5851931522810791E-2</v>
+      </c>
+      <c r="C332" s="9">
+        <v>0.44224765868887761</v>
+      </c>
+      <c r="D332" s="9">
+        <v>-1.1042944785276143</v>
+      </c>
+      <c r="E332" s="9">
+        <v>-0.29069767441860189</v>
+      </c>
+      <c r="F332" s="9">
+        <v>0.18975332068310116</v>
+      </c>
+      <c r="G332" s="9">
+        <v>0.96305031446540879</v>
+      </c>
+      <c r="H332" s="9">
+        <v>0.9624197983501479</v>
+      </c>
+      <c r="I332" s="9">
+        <v>-1.9165247018739351</v>
+      </c>
+      <c r="J332" s="9">
+        <v>-0.15060240963856705</v>
+      </c>
+      <c r="K332" s="9">
+        <v>-1.5282940933498508</v>
+      </c>
+      <c r="L332" s="9">
+        <v>0.52417532760957564</v>
+      </c>
+      <c r="M332" s="9">
+        <v>0.72918185795537405</v>
+      </c>
+      <c r="N332" s="9">
+        <v>-0.94711917916338018</v>
+      </c>
+      <c r="O332" s="9">
+        <v>3.0303030303030329</v>
+      </c>
+      <c r="P332" s="9">
+        <v>0.92771084337349952</v>
+      </c>
+      <c r="Q332" s="9">
+        <v>7.0339976553343814E-2</v>
+      </c>
+      <c r="R332" s="9">
+        <v>7.7071290944118936E-2</v>
+      </c>
+      <c r="S332" s="9">
+        <v>0.58616647127783184</v>
+      </c>
+      <c r="T332" s="9">
+        <v>-0.28481012658227128</v>
+      </c>
+      <c r="U332" s="9">
+        <v>-0.88414634146340776</v>
+      </c>
+      <c r="V332" s="9">
+        <v>0</v>
+      </c>
+      <c r="W332" s="9">
+        <v>-0.39572615749901069</v>
+      </c>
+      <c r="X332" s="9">
+        <v>-0.44208664898320071</v>
+      </c>
+      <c r="Y332" s="9">
+        <v>1.4157228514323783</v>
+      </c>
+      <c r="Z332" s="9">
+        <v>1.7102137767220877</v>
+      </c>
+      <c r="AA332" s="9">
+        <v>-0.12330456226880861</v>
+      </c>
+      <c r="AB332" s="9">
+        <v>0.13840830449827513</v>
+      </c>
+      <c r="AC332" s="9">
+        <v>0.9933774834437149</v>
+      </c>
+      <c r="AD332" s="9">
+        <v>5.7836899942159813E-2</v>
+      </c>
+      <c r="AE332" s="9">
+        <v>2.5657071339173929</v>
+      </c>
+      <c r="AF332" s="9">
+        <v>-0.22123893805310046</v>
+      </c>
+      <c r="AG332" s="9">
+        <v>0.29320736276267606</v>
+      </c>
+      <c r="AH332" s="9">
+        <v>0.21401819154628446</v>
+      </c>
+      <c r="AI332" s="9">
+        <v>7.5914423740504416E-2</v>
+      </c>
+      <c r="AJ332" s="9">
+        <v>0.80799780881949845</v>
+      </c>
+      <c r="AK332" s="9">
+        <v>-2.5362318840579641</v>
+      </c>
+      <c r="AL332" s="9">
+        <v>0.35696073431923359</v>
+      </c>
+      <c r="AM332" s="9">
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="AN332" s="9">
+        <v>-5.5966548729494949</v>
+      </c>
+      <c r="AO332" s="9">
+        <v>-0.29871977240398617</v>
+      </c>
+      <c r="AP332" s="9">
+        <v>0.33003300330032304</v>
+      </c>
+      <c r="AQ332" s="9">
+        <v>0.73992874760209526</v>
+      </c>
+      <c r="AR332" s="9">
+        <v>1.5209125475285026</v>
+      </c>
+      <c r="AS332" s="9">
+        <v>0.46554934823091243</v>
+      </c>
+      <c r="AT332" s="9">
+        <v>0.25763899623847064</v>
+      </c>
+      <c r="AU332" s="9">
+        <v>1.8121911037891174</v>
+      </c>
+      <c r="AV332" s="9">
+        <v>0.35906642728904081</v>
+      </c>
+      <c r="AW332" s="9">
+        <v>-4.1887740854519434E-2</v>
+      </c>
+      <c r="AX332" s="9">
+        <v>1.646937725167271</v>
+      </c>
+      <c r="AY332" s="9">
+        <v>-1.2795905310300704</v>
+      </c>
+      <c r="AZ332" s="9">
+        <v>0.5428077966938043</v>
+      </c>
+      <c r="BA332" s="9">
+        <v>-1.8465909090909252</v>
+      </c>
     </row>
     <row r="333" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A333" s="7"/>
+      <c r="A333" s="7">
+        <v>43191</v>
+      </c>
+      <c r="B333" s="9">
+        <v>1.3443871835088507E-2</v>
+      </c>
+      <c r="C333" s="9">
+        <v>0.4940197607904257</v>
+      </c>
+      <c r="D333" s="9">
+        <v>-1.1070110701106906</v>
+      </c>
+      <c r="E333" s="9">
+        <v>-0.24213075060532688</v>
+      </c>
+      <c r="F333" s="9">
+        <v>4.7348484848495617E-2</v>
+      </c>
+      <c r="G333" s="9">
+        <v>0.9626719056974461</v>
+      </c>
+      <c r="H333" s="9">
+        <v>1.3079394217530951</v>
+      </c>
+      <c r="I333" s="9">
+        <v>-0.98967297762478978</v>
+      </c>
+      <c r="J333" s="9">
+        <v>0.60422960725074237</v>
+      </c>
+      <c r="K333" s="9">
+        <v>-1.1608623548921986</v>
+      </c>
+      <c r="L333" s="9">
+        <v>0.72358900144717808</v>
+      </c>
+      <c r="M333" s="9">
+        <v>0.94793641534198625</v>
+      </c>
+      <c r="N333" s="9">
+        <v>-1.7268445839874433</v>
+      </c>
+      <c r="O333" s="9">
+        <v>2.6122448979591857</v>
+      </c>
+      <c r="P333" s="9">
+        <v>1.1741919864423112</v>
+      </c>
+      <c r="Q333" s="9">
+        <v>1.5899383009017669</v>
+      </c>
+      <c r="R333" s="9">
+        <v>0.15402387370043671</v>
+      </c>
+      <c r="S333" s="9">
+        <v>0.50721810378463184</v>
+      </c>
+      <c r="T333" s="9">
+        <v>-6.341154090044028E-2</v>
+      </c>
+      <c r="U333" s="9">
+        <v>-0.91268634012777616</v>
+      </c>
+      <c r="V333" s="9">
+        <v>0.40040040040039182</v>
+      </c>
+      <c r="W333" s="9">
+        <v>-0.65424266455193392</v>
+      </c>
+      <c r="X333" s="9">
+        <v>-0.22143489813994682</v>
+      </c>
+      <c r="Y333" s="9">
+        <v>1.296973727968086</v>
+      </c>
+      <c r="Z333" s="9">
+        <v>1.7577197149643651</v>
+      </c>
+      <c r="AA333" s="9">
+        <v>0.20635575732562939</v>
+      </c>
+      <c r="AB333" s="9">
+        <v>0.34618047542118624</v>
+      </c>
+      <c r="AC333" s="9">
+        <v>0.77177508269019057</v>
+      </c>
+      <c r="AD333" s="9">
+        <v>-0.17361111111111768</v>
+      </c>
+      <c r="AE333" s="9">
+        <v>3.0798240100565719</v>
+      </c>
+      <c r="AF333" s="9">
+        <v>-0.66445182724251861</v>
+      </c>
+      <c r="AG333" s="9">
+        <v>0.49043648847474253</v>
+      </c>
+      <c r="AH333" s="9">
+        <v>5.3447354355956336E-2</v>
+      </c>
+      <c r="AI333" s="9">
+        <v>0.1519337016574617</v>
+      </c>
+      <c r="AJ333" s="9">
+        <v>0.94481719841162415</v>
+      </c>
+      <c r="AK333" s="9">
+        <v>-2.5362318840579641</v>
+      </c>
+      <c r="AL333" s="9">
+        <v>0.58883768561186745</v>
+      </c>
+      <c r="AM333" s="9">
+        <v>0.48627002288329191</v>
+      </c>
+      <c r="AN333" s="9">
+        <v>-5.2002583979328234</v>
+      </c>
+      <c r="AO333" s="9">
+        <v>-0.3130781272235727</v>
+      </c>
+      <c r="AP333" s="9">
+        <v>0.16556291390728714</v>
+      </c>
+      <c r="AQ333" s="9">
+        <v>0.87767416346680971</v>
+      </c>
+      <c r="AR333" s="9">
+        <v>1.6455696202531609</v>
+      </c>
+      <c r="AS333" s="9">
+        <v>0.55852920642309389</v>
+      </c>
+      <c r="AT333" s="9">
+        <v>0.24709152681973551</v>
+      </c>
+      <c r="AU333" s="9">
+        <v>1.6872427983539071</v>
+      </c>
+      <c r="AV333" s="9">
+        <v>0.36036036036036551</v>
+      </c>
+      <c r="AW333" s="9">
+        <v>-0.19533975163947129</v>
+      </c>
+      <c r="AX333" s="9">
+        <v>1.4192886456908462</v>
+      </c>
+      <c r="AY333" s="9">
+        <v>-0.38935756002595351</v>
+      </c>
+      <c r="AZ333" s="9">
+        <v>0.44139283962727099</v>
+      </c>
+      <c r="BA333" s="9">
+        <v>-1.9858156028368874</v>
+      </c>
     </row>
     <row r="334" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A334" s="7"/>

</xml_diff>

<commit_message>
emp and earnings update
</commit_message>
<xml_diff>
--- a/data/historical/source/gov_employment_historical.xlsx
+++ b/data/historical/source/gov_employment_historical.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\Box Sync\TPC\CENTER\SLFI\SEM\Historical\Employment\PUBLISHED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EHuffer\AppData\Local\Box\Box Edit\Documents\x2Dk+Vb9g0qnP+BFeSxj2A==\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
@@ -186,7 +183,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Government Employment; Year/Year: January 1991 -- April 2018</t>
+    <t>Government Employment; Year/Year: January 1991 -- July 2018</t>
   </si>
 </sst>
 </file>
@@ -1376,670 +1373,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TABLE"/>
-      <sheetName val="FRED"/>
-      <sheetName val="fred1"/>
-      <sheetName val="fred2"/>
-      <sheetName val="fred3"/>
-      <sheetName val="fred4"/>
-      <sheetName val="KEY"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="336">
-          <cell r="B336">
-            <v>22305</v>
-          </cell>
-          <cell r="D336">
-            <v>81.7</v>
-          </cell>
-          <cell r="F336">
-            <v>384.8</v>
-          </cell>
-          <cell r="H336">
-            <v>211.2</v>
-          </cell>
-          <cell r="J336">
-            <v>413.1</v>
-          </cell>
-          <cell r="L336">
-            <v>2548.6999999999998</v>
-          </cell>
-          <cell r="N336">
-            <v>435.3</v>
-          </cell>
-          <cell r="P336">
-            <v>232.2</v>
-          </cell>
-          <cell r="R336">
-            <v>66.099999999999994</v>
-          </cell>
-          <cell r="T336">
-            <v>241.1</v>
-          </cell>
-          <cell r="V336">
-            <v>1105.9000000000001</v>
-          </cell>
-          <cell r="X336">
-            <v>685.3</v>
-          </cell>
-          <cell r="Z336">
-            <v>126.3</v>
-          </cell>
-          <cell r="AB336">
-            <v>259.2</v>
-          </cell>
-          <cell r="AD336">
-            <v>122.9</v>
-          </cell>
-          <cell r="AF336">
-            <v>824.2</v>
-          </cell>
-          <cell r="AH336">
-            <v>425</v>
-          </cell>
-          <cell r="AJ336">
-            <v>255.7</v>
-          </cell>
-          <cell r="AL336">
-            <v>316</v>
-          </cell>
-          <cell r="AN336">
-            <v>327.8</v>
-          </cell>
-          <cell r="AP336">
-            <v>452.1</v>
-          </cell>
-          <cell r="AR336">
-            <v>505.6</v>
-          </cell>
-          <cell r="AT336">
-            <v>100</v>
-          </cell>
-          <cell r="AV336">
-            <v>601.70000000000005</v>
-          </cell>
-          <cell r="AX336">
-            <v>421.8</v>
-          </cell>
-          <cell r="AZ336">
-            <v>434.3</v>
-          </cell>
-          <cell r="BB336">
-            <v>241.9</v>
-          </cell>
-          <cell r="BD336">
-            <v>90.6</v>
-          </cell>
-          <cell r="BF336">
-            <v>731.5</v>
-          </cell>
-          <cell r="BH336">
-            <v>82.7</v>
-          </cell>
-          <cell r="BJ336">
-            <v>172.7</v>
-          </cell>
-          <cell r="BL336">
-            <v>90.3</v>
-          </cell>
-          <cell r="BN336">
-            <v>612.5</v>
-          </cell>
-          <cell r="BP336">
-            <v>185.8</v>
-          </cell>
-          <cell r="BR336">
-            <v>159.9</v>
-          </cell>
-          <cell r="BT336">
-            <v>1447.4</v>
-          </cell>
-          <cell r="BV336">
-            <v>780.3</v>
-          </cell>
-          <cell r="BX336">
-            <v>349.5</v>
-          </cell>
-          <cell r="BZ336">
-            <v>309.60000000000002</v>
-          </cell>
-          <cell r="CB336">
-            <v>704</v>
-          </cell>
-          <cell r="CD336">
-            <v>60.5</v>
-          </cell>
-          <cell r="CF336">
-            <v>364.6</v>
-          </cell>
-          <cell r="CH336">
-            <v>79.5</v>
-          </cell>
-          <cell r="CJ336">
-            <v>429.7</v>
-          </cell>
-          <cell r="CL336">
-            <v>1941.4</v>
-          </cell>
-          <cell r="CN336">
-            <v>243.2</v>
-          </cell>
-          <cell r="CP336">
-            <v>716.8</v>
-          </cell>
-          <cell r="CR336">
-            <v>54.6</v>
-          </cell>
-          <cell r="CT336">
-            <v>585.9</v>
-          </cell>
-          <cell r="CV336">
-            <v>410.2</v>
-          </cell>
-          <cell r="CX336">
-            <v>153.80000000000001</v>
-          </cell>
-          <cell r="CZ336">
-            <v>70.5</v>
-          </cell>
-        </row>
-        <row r="337">
-          <cell r="B337">
-            <v>22324</v>
-          </cell>
-          <cell r="D337">
-            <v>81</v>
-          </cell>
-          <cell r="F337">
-            <v>385.3</v>
-          </cell>
-          <cell r="H337">
-            <v>211.7</v>
-          </cell>
-          <cell r="J337">
-            <v>414.3</v>
-          </cell>
-          <cell r="L337">
-            <v>2552</v>
-          </cell>
-          <cell r="N337">
-            <v>431.5</v>
-          </cell>
-          <cell r="P337">
-            <v>232.6</v>
-          </cell>
-          <cell r="R337">
-            <v>66.3</v>
-          </cell>
-          <cell r="T337">
-            <v>241</v>
-          </cell>
-          <cell r="V337">
-            <v>1106.8</v>
-          </cell>
-          <cell r="X337">
-            <v>687.6</v>
-          </cell>
-          <cell r="Z337">
-            <v>126</v>
-          </cell>
-          <cell r="AB337">
-            <v>260.39999999999998</v>
-          </cell>
-          <cell r="AD337">
-            <v>123.2</v>
-          </cell>
-          <cell r="AF337">
-            <v>832.8</v>
-          </cell>
-          <cell r="AH337">
-            <v>427.3</v>
-          </cell>
-          <cell r="AJ337">
-            <v>255.4</v>
-          </cell>
-          <cell r="AL337">
-            <v>315.7</v>
-          </cell>
-          <cell r="AN337">
-            <v>327.3</v>
-          </cell>
-          <cell r="AP337">
-            <v>454.3</v>
-          </cell>
-          <cell r="AR337">
-            <v>506.7</v>
-          </cell>
-          <cell r="AT337">
-            <v>100</v>
-          </cell>
-          <cell r="AV337">
-            <v>603.20000000000005</v>
-          </cell>
-          <cell r="AX337">
-            <v>420.7</v>
-          </cell>
-          <cell r="AZ337">
-            <v>436.4</v>
-          </cell>
-          <cell r="BB337">
-            <v>242</v>
-          </cell>
-          <cell r="BD337">
-            <v>91.3</v>
-          </cell>
-          <cell r="BF337">
-            <v>733.1</v>
-          </cell>
-          <cell r="BH337">
-            <v>82.7</v>
-          </cell>
-          <cell r="BJ337">
-            <v>172.9</v>
-          </cell>
-          <cell r="BL337">
-            <v>90.4</v>
-          </cell>
-          <cell r="BN337">
-            <v>614.79999999999995</v>
-          </cell>
-          <cell r="BP337">
-            <v>184.3</v>
-          </cell>
-          <cell r="BR337">
-            <v>160</v>
-          </cell>
-          <cell r="BT337">
-            <v>1448.1</v>
-          </cell>
-          <cell r="BV337">
-            <v>781.1</v>
-          </cell>
-          <cell r="BX337">
-            <v>349.8</v>
-          </cell>
-          <cell r="BZ337">
-            <v>309.8</v>
-          </cell>
-          <cell r="CB337">
-            <v>703.4</v>
-          </cell>
-          <cell r="CD337">
-            <v>60.8</v>
-          </cell>
-          <cell r="CF337">
-            <v>365</v>
-          </cell>
-          <cell r="CH337">
-            <v>78.900000000000006</v>
-          </cell>
-          <cell r="CJ337">
-            <v>430.3</v>
-          </cell>
-          <cell r="CL337">
-            <v>1939.3</v>
-          </cell>
-          <cell r="CN337">
-            <v>243.3</v>
-          </cell>
-          <cell r="CP337">
-            <v>717.8</v>
-          </cell>
-          <cell r="CR337">
-            <v>55.7</v>
-          </cell>
-          <cell r="CT337">
-            <v>587.6</v>
-          </cell>
-          <cell r="CV337">
-            <v>406.9</v>
-          </cell>
-          <cell r="CX337">
-            <v>153.69999999999999</v>
-          </cell>
-          <cell r="CZ337">
-            <v>70.3</v>
-          </cell>
-        </row>
-        <row r="348">
-          <cell r="A348">
-            <v>43221</v>
-          </cell>
-          <cell r="B348">
-            <v>22330</v>
-          </cell>
-          <cell r="D348">
-            <v>80.8</v>
-          </cell>
-          <cell r="F348">
-            <v>385.7</v>
-          </cell>
-          <cell r="H348">
-            <v>211.4</v>
-          </cell>
-          <cell r="J348">
-            <v>413.8</v>
-          </cell>
-          <cell r="L348">
-            <v>2571.6999999999998</v>
-          </cell>
-          <cell r="N348">
-            <v>442.3</v>
-          </cell>
-          <cell r="P348">
-            <v>229.6</v>
-          </cell>
-          <cell r="R348">
-            <v>66.5</v>
-          </cell>
-          <cell r="T348">
-            <v>238</v>
-          </cell>
-          <cell r="V348">
-            <v>1107.3</v>
-          </cell>
-          <cell r="X348">
-            <v>689.9</v>
-          </cell>
-          <cell r="Z348">
-            <v>125.8</v>
-          </cell>
-          <cell r="AB348">
-            <v>259.10000000000002</v>
-          </cell>
-          <cell r="AD348">
-            <v>125.8</v>
-          </cell>
-          <cell r="AF348">
-            <v>838.3</v>
-          </cell>
-          <cell r="AH348">
-            <v>427.2</v>
-          </cell>
-          <cell r="AJ348">
-            <v>257.7</v>
-          </cell>
-          <cell r="AL348">
-            <v>315</v>
-          </cell>
-          <cell r="AN348">
-            <v>324.89999999999998</v>
-          </cell>
-          <cell r="AP348">
-            <v>451.1</v>
-          </cell>
-          <cell r="AR348">
-            <v>503.8</v>
-          </cell>
-          <cell r="AT348">
-            <v>100.4</v>
-          </cell>
-          <cell r="AV348">
-            <v>607.4</v>
-          </cell>
-          <cell r="AX348">
-            <v>428.2</v>
-          </cell>
-          <cell r="AZ348">
-            <v>435.8</v>
-          </cell>
-          <cell r="BB348">
-            <v>242.1</v>
-          </cell>
-          <cell r="BD348">
-            <v>91.4</v>
-          </cell>
-          <cell r="BF348">
-            <v>736.4</v>
-          </cell>
-          <cell r="BH348">
-            <v>80.599999999999994</v>
-          </cell>
-          <cell r="BJ348">
-            <v>172.7</v>
-          </cell>
-          <cell r="BL348">
-            <v>90</v>
-          </cell>
-          <cell r="BN348">
-            <v>615.79999999999995</v>
-          </cell>
-          <cell r="BP348">
-            <v>184.7</v>
-          </cell>
-          <cell r="BR348">
-            <v>165.7</v>
-          </cell>
-          <cell r="BT348">
-            <v>1448.5</v>
-          </cell>
-          <cell r="BV348">
-            <v>785.5</v>
-          </cell>
-          <cell r="BX348">
-            <v>350.8</v>
-          </cell>
-          <cell r="BZ348">
-            <v>293.5</v>
-          </cell>
-          <cell r="CB348">
-            <v>702.2</v>
-          </cell>
-          <cell r="CD348">
-            <v>60.6</v>
-          </cell>
-          <cell r="CF348">
-            <v>368.1</v>
-          </cell>
-          <cell r="CH348">
-            <v>80.599999999999994</v>
-          </cell>
-          <cell r="CJ348">
-            <v>432.4</v>
-          </cell>
-          <cell r="CL348">
-            <v>1946.3</v>
-          </cell>
-          <cell r="CN348">
-            <v>247.5</v>
-          </cell>
-          <cell r="CP348">
-            <v>714.5</v>
-          </cell>
-          <cell r="CR348">
-            <v>55.3</v>
-          </cell>
-          <cell r="CT348">
-            <v>594</v>
-          </cell>
-          <cell r="CV348">
-            <v>409.1</v>
-          </cell>
-          <cell r="CX348">
-            <v>161.9</v>
-          </cell>
-          <cell r="CZ348">
-            <v>68.900000000000006</v>
-          </cell>
-        </row>
-        <row r="349">
-          <cell r="A349">
-            <v>43252</v>
-          </cell>
-          <cell r="B349">
-            <v>22341</v>
-          </cell>
-          <cell r="D349">
-            <v>80.3</v>
-          </cell>
-          <cell r="F349">
-            <v>388.5</v>
-          </cell>
-          <cell r="H349">
-            <v>211.4</v>
-          </cell>
-          <cell r="J349">
-            <v>414.4</v>
-          </cell>
-          <cell r="L349">
-            <v>2575.1999999999998</v>
-          </cell>
-          <cell r="N349">
-            <v>442.8</v>
-          </cell>
-          <cell r="P349">
-            <v>228.1</v>
-          </cell>
-          <cell r="R349">
-            <v>67.099999999999994</v>
-          </cell>
-          <cell r="T349">
-            <v>237.8</v>
-          </cell>
-          <cell r="V349">
-            <v>1104.7</v>
-          </cell>
-          <cell r="X349">
-            <v>691.7</v>
-          </cell>
-          <cell r="Z349">
-            <v>125.8</v>
-          </cell>
-          <cell r="AB349">
-            <v>262</v>
-          </cell>
-          <cell r="AD349">
-            <v>125.6</v>
-          </cell>
-          <cell r="AF349">
-            <v>845.7</v>
-          </cell>
-          <cell r="AH349">
-            <v>428</v>
-          </cell>
-          <cell r="AJ349">
-            <v>258</v>
-          </cell>
-          <cell r="AL349">
-            <v>314.2</v>
-          </cell>
-          <cell r="AN349">
-            <v>324.60000000000002</v>
-          </cell>
-          <cell r="AP349">
-            <v>454.3</v>
-          </cell>
-          <cell r="AR349">
-            <v>499.8</v>
-          </cell>
-          <cell r="AT349">
-            <v>100.5</v>
-          </cell>
-          <cell r="AV349">
-            <v>603.70000000000005</v>
-          </cell>
-          <cell r="AX349">
-            <v>427.2</v>
-          </cell>
-          <cell r="AZ349">
-            <v>436.5</v>
-          </cell>
-          <cell r="BB349">
-            <v>241</v>
-          </cell>
-          <cell r="BD349">
-            <v>91.2</v>
-          </cell>
-          <cell r="BF349">
-            <v>738.3</v>
-          </cell>
-          <cell r="BH349">
-            <v>80.5</v>
-          </cell>
-          <cell r="BJ349">
-            <v>172.8</v>
-          </cell>
-          <cell r="BL349">
-            <v>90.3</v>
-          </cell>
-          <cell r="BN349">
-            <v>616.6</v>
-          </cell>
-          <cell r="BP349">
-            <v>186.4</v>
-          </cell>
-          <cell r="BR349">
-            <v>166.7</v>
-          </cell>
-          <cell r="BT349">
-            <v>1449</v>
-          </cell>
-          <cell r="BV349">
-            <v>784.3</v>
-          </cell>
-          <cell r="BX349">
-            <v>351</v>
-          </cell>
-          <cell r="BZ349">
-            <v>293.8</v>
-          </cell>
-          <cell r="CB349">
-            <v>701.5</v>
-          </cell>
-          <cell r="CD349">
-            <v>60.5</v>
-          </cell>
-          <cell r="CF349">
-            <v>368.6</v>
-          </cell>
-          <cell r="CH349">
-            <v>79.8</v>
-          </cell>
-          <cell r="CJ349">
-            <v>432.5</v>
-          </cell>
-          <cell r="CL349">
-            <v>1947.1</v>
-          </cell>
-          <cell r="CN349">
-            <v>247.5</v>
-          </cell>
-          <cell r="CP349">
-            <v>712.3</v>
-          </cell>
-          <cell r="CR349">
-            <v>55.7</v>
-          </cell>
-          <cell r="CT349">
-            <v>593.29999999999995</v>
-          </cell>
-          <cell r="CV349">
-            <v>411</v>
-          </cell>
-          <cell r="CX349">
-            <v>154.6</v>
-          </cell>
-          <cell r="CZ349">
-            <v>68.8</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2364,8 +1697,8 @@
   <dimension ref="A1:BA590"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B338" sqref="B338"/>
+      <pane ySplit="5" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A337" sqref="A337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -55038,7 +54371,7 @@
         <v>43160</v>
       </c>
       <c r="B332" s="9">
-        <v>3.5851931522810791E-2</v>
+        <v>4.4814914403513491E-2</v>
       </c>
       <c r="C332" s="9">
         <v>0.44224765868887761</v>
@@ -55199,25 +54532,25 @@
         <v>43191</v>
       </c>
       <c r="B333" s="9">
-        <v>1.3443871835088507E-2</v>
+        <v>4.4812906116961683E-2</v>
       </c>
       <c r="C333" s="9">
-        <v>0.4940197607904257</v>
+        <v>0.4420176807072253</v>
       </c>
       <c r="D333" s="9">
-        <v>-1.1070110701106906</v>
+        <v>-0.98400984009839754</v>
       </c>
       <c r="E333" s="9">
-        <v>-0.24213075060532688</v>
+        <v>-4.8426150121062619E-2</v>
       </c>
       <c r="F333" s="9">
         <v>4.7348484848495617E-2</v>
       </c>
       <c r="G333" s="9">
-        <v>0.9626719056974461</v>
+        <v>0.95088408644400069</v>
       </c>
       <c r="H333" s="9">
-        <v>1.3079394217530951</v>
+        <v>1.3538320330426747</v>
       </c>
       <c r="I333" s="9">
         <v>-0.98967297762478978</v>
@@ -55226,28 +54559,28 @@
         <v>0.60422960725074237</v>
       </c>
       <c r="K333" s="9">
-        <v>-1.1608623548921986</v>
+        <v>-1.326699834162516</v>
       </c>
       <c r="L333" s="9">
-        <v>0.72358900144717808</v>
+        <v>0.48842257597685346</v>
       </c>
       <c r="M333" s="9">
-        <v>0.94793641534198625</v>
+        <v>0.80210004375091148</v>
       </c>
       <c r="N333" s="9">
         <v>-1.7268445839874433</v>
       </c>
       <c r="O333" s="9">
-        <v>2.6122448979591857</v>
+        <v>2.5306122448979544</v>
       </c>
       <c r="P333" s="9">
-        <v>1.1741919864423112</v>
+        <v>1.1257716983415995</v>
       </c>
       <c r="Q333" s="9">
-        <v>1.5899383009017669</v>
+        <v>1.7560512577123952</v>
       </c>
       <c r="R333" s="9">
-        <v>0.15402387370043671</v>
+        <v>0</v>
       </c>
       <c r="S333" s="9">
         <v>0.50721810378463184</v>
@@ -55259,25 +54592,25 @@
         <v>-0.91268634012777616</v>
       </c>
       <c r="V333" s="9">
-        <v>0.40040040040039182</v>
+        <v>0.50050050050050054</v>
       </c>
       <c r="W333" s="9">
-        <v>-0.65424266455193392</v>
+        <v>-0.57494052339412716</v>
       </c>
       <c r="X333" s="9">
         <v>-0.22143489813994682</v>
       </c>
       <c r="Y333" s="9">
-        <v>1.296973727968086</v>
+        <v>1.0142999667442671</v>
       </c>
       <c r="Z333" s="9">
         <v>1.7577197149643651</v>
       </c>
       <c r="AA333" s="9">
-        <v>0.20635575732562939</v>
+        <v>0.16508460586049412</v>
       </c>
       <c r="AB333" s="9">
-        <v>0.34618047542118624</v>
+        <v>0.39233787214400845</v>
       </c>
       <c r="AC333" s="9">
         <v>0.77177508269019057</v>
@@ -55286,28 +54619,28 @@
         <v>-0.17361111111111768</v>
       </c>
       <c r="AE333" s="9">
-        <v>3.0798240100565719</v>
+        <v>4.0854808296668761</v>
       </c>
       <c r="AF333" s="9">
-        <v>-0.66445182724251861</v>
+        <v>-0.55370985603543743</v>
       </c>
       <c r="AG333" s="9">
-        <v>0.49043648847474253</v>
+        <v>0.50678437142388566</v>
       </c>
       <c r="AH333" s="9">
-        <v>5.3447354355956336E-2</v>
+        <v>0.10689470871192788</v>
       </c>
       <c r="AI333" s="9">
-        <v>0.1519337016574617</v>
+        <v>0.11740331491713021</v>
       </c>
       <c r="AJ333" s="9">
-        <v>0.94481719841162415</v>
+        <v>0.84896617828290366</v>
       </c>
       <c r="AK333" s="9">
-        <v>-2.5362318840579641</v>
+        <v>-2.6570048309178778</v>
       </c>
       <c r="AL333" s="9">
-        <v>0.58883768561186745</v>
+        <v>0.53763440860214173</v>
       </c>
       <c r="AM333" s="9">
         <v>0.48627002288329191</v>
@@ -55316,22 +54649,22 @@
         <v>-5.2002583979328234</v>
       </c>
       <c r="AO333" s="9">
-        <v>-0.3130781272235727</v>
+        <v>-0.41269389497653203</v>
       </c>
       <c r="AP333" s="9">
         <v>0.16556291390728714</v>
       </c>
       <c r="AQ333" s="9">
-        <v>0.87767416346680971</v>
+        <v>0.85024684585846555</v>
       </c>
       <c r="AR333" s="9">
-        <v>1.6455696202531609</v>
+        <v>2.0253164556961951</v>
       </c>
       <c r="AS333" s="9">
-        <v>0.55852920642309389</v>
+        <v>0.60507330695834827</v>
       </c>
       <c r="AT333" s="9">
-        <v>0.24709152681973551</v>
+        <v>0.21620508596726273</v>
       </c>
       <c r="AU333" s="9">
         <v>1.6872427983539071</v>
@@ -55340,451 +54673,503 @@
         <v>0.36036036036036551</v>
       </c>
       <c r="AW333" s="9">
-        <v>-0.19533975163947129</v>
+        <v>-0.18138691223664966</v>
       </c>
       <c r="AX333" s="9">
-        <v>1.4192886456908462</v>
+        <v>1.4363885088919444</v>
       </c>
       <c r="AY333" s="9">
-        <v>-0.38935756002595351</v>
+        <v>-0.45425048669694268</v>
       </c>
       <c r="AZ333" s="9">
-        <v>0.44139283962727099</v>
+        <v>9.8087297694942913E-2</v>
       </c>
       <c r="BA333" s="9">
-        <v>-1.9858156028368874</v>
+        <v>-1.7021276595744723</v>
       </c>
     </row>
     <row r="334" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A334" s="10">
-        <f>[1]FRED!A348</f>
         <v>43221</v>
       </c>
       <c r="B334" s="11">
-        <f>(([1]FRED!B348-[1]FRED!B336)/[1]FRED!B336)*100</f>
-        <v>0.11208249271463797</v>
+        <v>0.12553239184039452</v>
       </c>
       <c r="C334" s="11">
-        <f>(([1]FRED!F348-[1]FRED!F336)/[1]FRED!F336)*100</f>
         <v>0.23388773388772796</v>
       </c>
       <c r="D334" s="11">
-        <f>(([1]FRED!D348-[1]FRED!D336)/[1]FRED!D336)*100</f>
         <v>-1.1015911872705086</v>
       </c>
       <c r="E334" s="11">
-        <f>(([1]FRED!J348-[1]FRED!J336)/[1]FRED!J336)*100</f>
         <v>0.16945049624787911</v>
       </c>
       <c r="F334" s="11">
-        <f>(([1]FRED!H348-[1]FRED!H336)/[1]FRED!H336)*100</f>
         <v>9.4696969696977773E-2</v>
       </c>
       <c r="G334" s="11">
-        <f>(([1]FRED!L348-[1]FRED!L336)/[1]FRED!L336)*100</f>
         <v>0.90242084199788131</v>
       </c>
       <c r="H334" s="11">
-        <f>(([1]FRED!N348-[1]FRED!N336)/[1]FRED!N336)*100</f>
         <v>1.6080863772111189</v>
       </c>
       <c r="I334" s="11">
-        <f>(([1]FRED!P348-[1]FRED!P336)/[1]FRED!P336)*100</f>
         <v>-1.1197243755383268</v>
       </c>
       <c r="J334" s="11">
-        <f>(([1]FRED!R348-[1]FRED!R336)/[1]FRED!R336)*100</f>
         <v>0.60514372163389674</v>
       </c>
       <c r="K334" s="11">
-        <f>(([1]FRED!T348-[1]FRED!T336)/[1]FRED!T336)*100</f>
         <v>-1.2857735379510553</v>
       </c>
       <c r="L334" s="11">
-        <f>(([1]FRED!V348-[1]FRED!V336)/[1]FRED!V336)*100</f>
         <v>0.12659372456821263</v>
       </c>
       <c r="M334" s="11">
-        <f>(([1]FRED!X348-[1]FRED!X336)/[1]FRED!X336)*100</f>
         <v>0.67123887348606792</v>
       </c>
       <c r="N334" s="11">
-        <f>(([1]FRED!Z348-[1]FRED!Z336)/[1]FRED!Z336)*100</f>
         <v>-0.3958828186856691</v>
       </c>
       <c r="O334" s="11">
-        <f>(([1]FRED!AD348-[1]FRED!AD336)/[1]FRED!AD336)*100</f>
         <v>2.3596419853539392</v>
       </c>
       <c r="P334" s="11">
-        <f>(([1]FRED!AF348-[1]FRED!AF336)/[1]FRED!AF336)*100</f>
         <v>1.7107498180053273</v>
       </c>
       <c r="Q334" s="11">
-        <f>(([1]FRED!AH348-[1]FRED!AH336)/[1]FRED!AH336)*100</f>
         <v>0.5176470588235268</v>
       </c>
       <c r="R334" s="11">
-        <f>(([1]FRED!AB348-[1]FRED!AB336)/[1]FRED!AB336)*100</f>
         <v>-3.8580246913567089E-2</v>
       </c>
       <c r="S334" s="11">
-        <f>(([1]FRED!AJ348-[1]FRED!AJ336)/[1]FRED!AJ336)*100</f>
         <v>0.78216660148611661</v>
       </c>
       <c r="T334" s="11">
-        <f>(([1]FRED!AL348-[1]FRED!AL336)/[1]FRED!AL336)*100</f>
         <v>-0.31645569620253167</v>
       </c>
       <c r="U334" s="11">
-        <f>(([1]FRED!AN348-[1]FRED!AN336)/[1]FRED!AN336)*100</f>
         <v>-0.88468578401465359</v>
       </c>
       <c r="V334" s="11">
-        <f>(([1]FRED!AT348-[1]FRED!AT336)/[1]FRED!AT336)*100</f>
         <v>0.40000000000000563</v>
       </c>
       <c r="W334" s="11">
-        <f>(([1]FRED!AR348-[1]FRED!AR336)/[1]FRED!AR336)*100</f>
         <v>-0.35601265822785033</v>
       </c>
       <c r="X334" s="11">
-        <f>(([1]FRED!AP348-[1]FRED!AP336)/[1]FRED!AP336)*100</f>
         <v>-0.22119000221189999</v>
       </c>
       <c r="Y334" s="11">
-        <f>(([1]FRED!AV348-[1]FRED!AV336)/[1]FRED!AV336)*100</f>
         <v>0.94731593817515891</v>
       </c>
       <c r="Z334" s="11">
-        <f>(([1]FRED!AX348-[1]FRED!AX336)/[1]FRED!AX336)*100</f>
         <v>1.5173067804646698</v>
       </c>
       <c r="AA334" s="11">
-        <f>(([1]FRED!BB348-[1]FRED!BB336)/[1]FRED!BB336)*100</f>
         <v>8.2678792889619115E-2</v>
       </c>
       <c r="AB334" s="11">
-        <f>(([1]FRED!AZ348-[1]FRED!AZ336)/[1]FRED!AZ336)*100</f>
         <v>0.345383375546857</v>
       </c>
       <c r="AC334" s="11">
-        <f>(([1]FRED!BD348-[1]FRED!BD336)/[1]FRED!BD336)*100</f>
         <v>0.88300220750553138</v>
       </c>
       <c r="AD334" s="11">
-        <f>(([1]FRED!BJ348-[1]FRED!BJ336)/[1]FRED!BJ336)*100</f>
         <v>0</v>
       </c>
       <c r="AE334" s="11">
-        <f>(([1]FRED!BR348-[1]FRED!BR336)/[1]FRED!BR336)*100</f>
         <v>3.6272670419011774</v>
       </c>
       <c r="AF334" s="11">
-        <f>(([1]FRED!BL348-[1]FRED!BL336)/[1]FRED!BL336)*100</f>
         <v>-0.33222591362125931</v>
       </c>
       <c r="AG334" s="11">
-        <f>(([1]FRED!BN348-[1]FRED!BN336)/[1]FRED!BN336)*100</f>
         <v>0.53877551020407422</v>
       </c>
       <c r="AH334" s="11">
-        <f>(([1]FRED!BP348-[1]FRED!BP336)/[1]FRED!BP336)*100</f>
         <v>-0.5920344456404858</v>
       </c>
       <c r="AI334" s="11">
-        <f>(([1]FRED!BT348-[1]FRED!BT336)/[1]FRED!BT336)*100</f>
         <v>7.5998341854353252E-2</v>
       </c>
       <c r="AJ334" s="11">
-        <f>(([1]FRED!BF348-[1]FRED!BF336)/[1]FRED!BF336)*100</f>
         <v>0.66985645933014037</v>
       </c>
       <c r="AK334" s="11">
-        <f>(([1]FRED!BH348-[1]FRED!BH336)/[1]FRED!BH336)*100</f>
         <v>-2.539298669891183</v>
       </c>
       <c r="AL334" s="11">
-        <f>(([1]FRED!BV348-[1]FRED!BV336)/[1]FRED!BV336)*100</f>
         <v>0.66641035499167578</v>
       </c>
       <c r="AM334" s="11">
-        <f>(([1]FRED!BX348-[1]FRED!BX336)/[1]FRED!BX336)*100</f>
         <v>0.37195994277539668</v>
       </c>
       <c r="AN334" s="11">
-        <f>(([1]FRED!BZ348-[1]FRED!BZ336)/[1]FRED!BZ336)*100</f>
         <v>-5.2002583979328234</v>
       </c>
       <c r="AO334" s="11">
-        <f>(([1]FRED!CB348-[1]FRED!CB336)/[1]FRED!CB336)*100</f>
         <v>-0.25568181818181174</v>
       </c>
       <c r="AP334" s="11">
-        <f>(([1]FRED!CD348-[1]FRED!CD336)/[1]FRED!CD336)*100</f>
         <v>0.16528925619834947</v>
       </c>
       <c r="AQ334" s="11">
-        <f>(([1]FRED!CF348-[1]FRED!CF336)/[1]FRED!CF336)*100</f>
         <v>0.95995611629182653</v>
       </c>
       <c r="AR334" s="11">
-        <f>(([1]FRED!CH348-[1]FRED!CH336)/[1]FRED!CH336)*100</f>
         <v>1.3836477987421314</v>
       </c>
       <c r="AS334" s="11">
-        <f>(([1]FRED!CJ348-[1]FRED!CJ336)/[1]FRED!CJ336)*100</f>
         <v>0.62834535722596896</v>
       </c>
       <c r="AT334" s="11">
-        <f>(([1]FRED!CL348-[1]FRED!CL336)/[1]FRED!CL336)*100</f>
         <v>0.25239517873698691</v>
       </c>
       <c r="AU334" s="11">
-        <f>(([1]FRED!CN348-[1]FRED!CN336)/[1]FRED!CN336)*100</f>
         <v>1.7680921052631626</v>
       </c>
       <c r="AV334" s="11">
-        <f>(([1]FRED!CR348-[1]FRED!CR336)/[1]FRED!CR336)*100</f>
         <v>1.2820512820512742</v>
       </c>
       <c r="AW334" s="11">
-        <f>(([1]FRED!CP348-[1]FRED!CP336)/[1]FRED!CP336)*100</f>
         <v>-0.32087053571427937</v>
       </c>
       <c r="AX334" s="11">
-        <f>(([1]FRED!CT348-[1]FRED!CT336)/[1]FRED!CT336)*100</f>
         <v>1.3824884792626768</v>
       </c>
       <c r="AY334" s="11">
-        <f>(([1]FRED!CX348-[1]FRED!CX336)/[1]FRED!CX336)*100</f>
         <v>5.2665799739921937</v>
       </c>
       <c r="AZ334" s="11">
-        <f>(([1]FRED!CV348-[1]FRED!CV336)/[1]FRED!CV336)*100</f>
         <v>-0.2681618722574271</v>
       </c>
       <c r="BA334" s="11">
-        <f>(([1]FRED!CZ348-[1]FRED!CZ336)/[1]FRED!CZ336)*100</f>
         <v>-2.2695035460992825</v>
       </c>
     </row>
     <row r="335" spans="1:53" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A335" s="10">
-        <f>[1]FRED!A349</f>
         <v>43252</v>
       </c>
       <c r="B335" s="11">
-        <f>(([1]FRED!B349-[1]FRED!B337)/[1]FRED!B337)*100</f>
-        <v>7.6151227378605982E-2</v>
+        <v>0.10302813115929045</v>
       </c>
       <c r="C335" s="11">
-        <f>(([1]FRED!F349-[1]FRED!F337)/[1]FRED!F337)*100</f>
-        <v>0.83052167142486066</v>
+        <v>-0.28549182455230282</v>
       </c>
       <c r="D335" s="11">
-        <f>(([1]FRED!D349-[1]FRED!D337)/[1]FRED!D337)*100</f>
         <v>-0.86419753086420115</v>
       </c>
       <c r="E335" s="11">
-        <f>(([1]FRED!J349-[1]FRED!J337)/[1]FRED!J337)*100</f>
-        <v>2.4137098720725534E-2</v>
+        <v>0.21723388848659841</v>
       </c>
       <c r="F335" s="11">
-        <f>(([1]FRED!H349-[1]FRED!H337)/[1]FRED!H337)*100</f>
-        <v>-0.14170996693433302</v>
+        <v>-9.4473311289555342E-2</v>
       </c>
       <c r="G335" s="11">
-        <f>(([1]FRED!L349-[1]FRED!L337)/[1]FRED!L337)*100</f>
-        <v>0.90909090909090196</v>
+        <v>1.3087774294670882</v>
       </c>
       <c r="H335" s="11">
-        <f>(([1]FRED!N349-[1]FRED!N337)/[1]FRED!N337)*100</f>
-        <v>2.6187717265353445</v>
+        <v>3.4067207415990701</v>
       </c>
       <c r="I335" s="11">
-        <f>(([1]FRED!P349-[1]FRED!P337)/[1]FRED!P337)*100</f>
-        <v>-1.9346517626827171</v>
+        <v>-1.9776440240756639</v>
       </c>
       <c r="J335" s="11">
-        <f>(([1]FRED!R349-[1]FRED!R337)/[1]FRED!R337)*100</f>
-        <v>1.2066365007541435</v>
+        <v>0.60331825037708253</v>
       </c>
       <c r="K335" s="11">
-        <f>(([1]FRED!T349-[1]FRED!T337)/[1]FRED!T337)*100</f>
-        <v>-1.327800829875514</v>
+        <v>-1.4107883817427409</v>
       </c>
       <c r="L335" s="11">
-        <f>(([1]FRED!V349-[1]FRED!V337)/[1]FRED!V337)*100</f>
         <v>-0.18973617636428525</v>
       </c>
       <c r="M335" s="11">
-        <f>(([1]FRED!X349-[1]FRED!X337)/[1]FRED!X337)*100</f>
-        <v>0.59627690517743204</v>
+        <v>0.5090168702734148</v>
       </c>
       <c r="N335" s="11">
-        <f>(([1]FRED!Z349-[1]FRED!Z337)/[1]FRED!Z337)*100</f>
-        <v>-0.158730158730161</v>
+        <v>-0.31746031746032199</v>
       </c>
       <c r="O335" s="11">
-        <f>(([1]FRED!AD349-[1]FRED!AD337)/[1]FRED!AD337)*100</f>
-        <v>1.9480519480519412</v>
+        <v>2.7597402597402527</v>
       </c>
       <c r="P335" s="11">
-        <f>(([1]FRED!AF349-[1]FRED!AF337)/[1]FRED!AF337)*100</f>
-        <v>1.5489913544668699</v>
+        <v>1.5850144092219076</v>
       </c>
       <c r="Q335" s="11">
-        <f>(([1]FRED!AH349-[1]FRED!AH337)/[1]FRED!AH337)*100</f>
-        <v>0.1638193306810177</v>
+        <v>-1.0765270301895677</v>
       </c>
       <c r="R335" s="11">
-        <f>(([1]FRED!AB349-[1]FRED!AB337)/[1]FRED!AB337)*100</f>
-        <v>0.61443932411675228</v>
+        <v>1.0368663594470222</v>
       </c>
       <c r="S335" s="11">
-        <f>(([1]FRED!AJ349-[1]FRED!AJ337)/[1]FRED!AJ337)*100</f>
-        <v>1.0180109631949861</v>
+        <v>0.86139389193422755</v>
       </c>
       <c r="T335" s="11">
-        <f>(([1]FRED!AL349-[1]FRED!AL337)/[1]FRED!AL337)*100</f>
-        <v>-0.47513462147608487</v>
+        <v>-0.31675641431738993</v>
       </c>
       <c r="U335" s="11">
-        <f>(([1]FRED!AN349-[1]FRED!AN337)/[1]FRED!AN337)*100</f>
         <v>-0.82493125572868575</v>
       </c>
       <c r="V335" s="11">
-        <f>(([1]FRED!AT349-[1]FRED!AT337)/[1]FRED!AT337)*100</f>
-        <v>0.5</v>
+        <v>0.70000000000000284</v>
       </c>
       <c r="W335" s="11">
-        <f>(([1]FRED!AR349-[1]FRED!AR337)/[1]FRED!AR337)*100</f>
-        <v>-1.3617525162818191</v>
+        <v>-1.440694691138743</v>
       </c>
       <c r="X335" s="11">
-        <f>(([1]FRED!AP349-[1]FRED!AP337)/[1]FRED!AP337)*100</f>
+        <v>2.2011886418658571E-2</v>
+      </c>
+      <c r="Y335" s="11">
+        <v>6.6312997347476324E-2</v>
+      </c>
+      <c r="Z335" s="11">
+        <v>1.4975041597337797</v>
+      </c>
+      <c r="AA335" s="11">
+        <v>0.20661157024793389</v>
+      </c>
+      <c r="AB335" s="11">
+        <v>-4.5829514207146801E-2</v>
+      </c>
+      <c r="AC335" s="11">
+        <v>0.98576122672508848</v>
+      </c>
+      <c r="AD335" s="11">
+        <v>-0.23134759976865568</v>
+      </c>
+      <c r="AE335" s="11">
+        <v>4.375</v>
+      </c>
+      <c r="AF335" s="11">
+        <v>-0.33185840707965858</v>
+      </c>
+      <c r="AG335" s="11">
+        <v>0.27651268705270748</v>
+      </c>
+      <c r="AH335" s="11">
+        <v>0.70537167661420663</v>
+      </c>
+      <c r="AI335" s="11">
+        <v>7.5961604861552137E-2</v>
+      </c>
+      <c r="AJ335" s="11">
+        <v>0.83208293547947387</v>
+      </c>
+      <c r="AK335" s="11">
+        <v>-2.539298669891183</v>
+      </c>
+      <c r="AL335" s="11">
+        <v>0.75534502624503619</v>
+      </c>
+      <c r="AM335" s="11">
+        <v>0.42881646655231564</v>
+      </c>
+      <c r="AN335" s="11">
+        <v>-5.1969012265978121</v>
+      </c>
+      <c r="AO335" s="11">
+        <v>-0.29854990048336977</v>
+      </c>
+      <c r="AP335" s="11">
+        <v>-0.49342105263157432</v>
+      </c>
+      <c r="AQ335" s="11">
+        <v>0.82191780821917804</v>
+      </c>
+      <c r="AR335" s="11">
+        <v>1.013941698352341</v>
+      </c>
+      <c r="AS335" s="11">
+        <v>0.37183360446199532</v>
+      </c>
+      <c r="AT335" s="11">
+        <v>0.30938998607745061</v>
+      </c>
+      <c r="AU335" s="11">
+        <v>1.9317714755445903</v>
+      </c>
+      <c r="AV335" s="11">
+        <v>0.17953321364451402</v>
+      </c>
+      <c r="AW335" s="11">
+        <v>-0.69657286152131526</v>
+      </c>
+      <c r="AX335" s="11">
+        <v>1.0211027910142954</v>
+      </c>
+      <c r="AY335" s="11">
+        <v>0.52049446974626634</v>
+      </c>
+      <c r="AZ335" s="11">
+        <v>0.7618579503563585</v>
+      </c>
+      <c r="BA335" s="11">
+        <v>-2.1337126600284497</v>
+      </c>
+    </row>
+    <row r="336" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A336" s="7">
+        <v>43282</v>
+      </c>
+      <c r="B336" s="9">
+        <v>3.5832661470930754E-2</v>
+      </c>
+      <c r="C336" s="9">
+        <v>-0.49312224240852165</v>
+      </c>
+      <c r="D336" s="9">
+        <v>-0.61957868649318459</v>
+      </c>
+      <c r="E336" s="9">
+        <v>-2.4084778420030324E-2</v>
+      </c>
+      <c r="F336" s="9">
+        <v>-0.23573785950023576</v>
+      </c>
+      <c r="G336" s="9">
+        <v>1.3046033300685673</v>
+      </c>
+      <c r="H336" s="9">
+        <v>2.2217132386623888</v>
+      </c>
+      <c r="I336" s="9">
+        <v>-1.6407599309153638</v>
+      </c>
+      <c r="J336" s="9">
+        <v>0.60514372163389674</v>
+      </c>
+      <c r="K336" s="9">
+        <v>-0.62893081761006298</v>
+      </c>
+      <c r="L336" s="9">
+        <v>-7.2293511657324644E-2</v>
+      </c>
+      <c r="M336" s="9">
+        <v>-0.33328503115491498</v>
+      </c>
+      <c r="N336" s="9">
+        <v>0.9615384615384639</v>
+      </c>
+      <c r="O336" s="9">
+        <v>3.0844155844155821</v>
+      </c>
+      <c r="P336" s="9">
+        <v>1.3808837656099904</v>
+      </c>
+      <c r="Q336" s="9">
+        <v>-1.3849765258215909</v>
+      </c>
+      <c r="R336" s="9">
+        <v>0.15267175572518216</v>
+      </c>
+      <c r="S336" s="9">
+        <v>0.97694411879639365</v>
+      </c>
+      <c r="T336" s="9">
+        <v>-0.4420587306599234</v>
+      </c>
+      <c r="U336" s="9">
+        <v>-0.82644628099173212</v>
+      </c>
+      <c r="V336" s="9">
+        <v>0.29910269192422445</v>
+      </c>
+      <c r="W336" s="9">
+        <v>-0.53497127006142042</v>
+      </c>
+      <c r="X336" s="9">
+        <v>-2.2055580061748101E-2</v>
+      </c>
+      <c r="Y336" s="9">
+        <v>0.24867374005305037</v>
+      </c>
+      <c r="Z336" s="9">
+        <v>1.0352941176470536</v>
+      </c>
+      <c r="AA336" s="9">
         <v>0</v>
       </c>
-      <c r="Y335" s="11">
-        <f>(([1]FRED!AV349-[1]FRED!AV337)/[1]FRED!AV337)*100</f>
-        <v>8.289124668435012E-2</v>
-      </c>
-      <c r="Z335" s="11">
-        <f>(([1]FRED!AX349-[1]FRED!AX337)/[1]FRED!AX337)*100</f>
-        <v>1.5450439743285</v>
-      </c>
-      <c r="AA335" s="11">
-        <f>(([1]FRED!BB349-[1]FRED!BB337)/[1]FRED!BB337)*100</f>
-        <v>-0.41322314049586778</v>
-      </c>
-      <c r="AB335" s="11">
-        <f>(([1]FRED!AZ349-[1]FRED!AZ337)/[1]FRED!AZ337)*100</f>
-        <v>2.2914757103579913E-2</v>
-      </c>
-      <c r="AC335" s="11">
-        <f>(([1]FRED!BD349-[1]FRED!BD337)/[1]FRED!BD337)*100</f>
-        <v>-0.10952902519166957</v>
-      </c>
-      <c r="AD335" s="11">
-        <f>(([1]FRED!BJ349-[1]FRED!BJ337)/[1]FRED!BJ337)*100</f>
-        <v>-5.7836899942159813E-2</v>
-      </c>
-      <c r="AE335" s="11">
-        <f>(([1]FRED!BR349-[1]FRED!BR337)/[1]FRED!BR337)*100</f>
-        <v>4.1874999999999929</v>
-      </c>
-      <c r="AF335" s="11">
-        <f>(([1]FRED!BL349-[1]FRED!BL337)/[1]FRED!BL337)*100</f>
-        <v>-0.1106194690265581</v>
-      </c>
-      <c r="AG335" s="11">
-        <f>(([1]FRED!BN349-[1]FRED!BN337)/[1]FRED!BN337)*100</f>
-        <v>0.2927781392322818</v>
-      </c>
-      <c r="AH335" s="11">
-        <f>(([1]FRED!BP349-[1]FRED!BP337)/[1]FRED!BP337)*100</f>
-        <v>1.1394465545306534</v>
-      </c>
-      <c r="AI335" s="11">
-        <f>(([1]FRED!BT349-[1]FRED!BT337)/[1]FRED!BT337)*100</f>
-        <v>6.2150403977632142E-2</v>
-      </c>
-      <c r="AJ335" s="11">
-        <f>(([1]FRED!BF349-[1]FRED!BF337)/[1]FRED!BF337)*100</f>
-        <v>0.70931660073658875</v>
-      </c>
-      <c r="AK335" s="11">
-        <f>(([1]FRED!BH349-[1]FRED!BH337)/[1]FRED!BH337)*100</f>
-        <v>-2.6602176541717082</v>
-      </c>
-      <c r="AL335" s="11">
-        <f>(([1]FRED!BV349-[1]FRED!BV337)/[1]FRED!BV337)*100</f>
-        <v>0.40967865830238531</v>
-      </c>
-      <c r="AM335" s="11">
-        <f>(([1]FRED!BX349-[1]FRED!BX337)/[1]FRED!BX337)*100</f>
-        <v>0.34305317324184925</v>
-      </c>
-      <c r="AN335" s="11">
-        <f>(([1]FRED!BZ349-[1]FRED!BZ337)/[1]FRED!BZ337)*100</f>
-        <v>-5.1646223369916076</v>
-      </c>
-      <c r="AO335" s="11">
-        <f>(([1]FRED!CB349-[1]FRED!CB337)/[1]FRED!CB337)*100</f>
-        <v>-0.27011657662780453</v>
-      </c>
-      <c r="AP335" s="11">
-        <f>(([1]FRED!CD349-[1]FRED!CD337)/[1]FRED!CD337)*100</f>
-        <v>-0.49342105263157432</v>
-      </c>
-      <c r="AQ335" s="11">
-        <f>(([1]FRED!CF349-[1]FRED!CF337)/[1]FRED!CF337)*100</f>
-        <v>0.98630136986301986</v>
-      </c>
-      <c r="AR335" s="11">
-        <f>(([1]FRED!CH349-[1]FRED!CH337)/[1]FRED!CH337)*100</f>
-        <v>1.1406844106463769</v>
-      </c>
-      <c r="AS335" s="11">
-        <f>(([1]FRED!CJ349-[1]FRED!CJ337)/[1]FRED!CJ337)*100</f>
-        <v>0.51127120613525179</v>
-      </c>
-      <c r="AT335" s="11">
-        <f>(([1]FRED!CL349-[1]FRED!CL337)/[1]FRED!CL337)*100</f>
-        <v>0.40220698190068349</v>
-      </c>
-      <c r="AU335" s="11">
-        <f>(([1]FRED!CN349-[1]FRED!CN337)/[1]FRED!CN337)*100</f>
-        <v>1.7262638717632506</v>
-      </c>
-      <c r="AV335" s="11">
-        <f>(([1]FRED!CR349-[1]FRED!CR337)/[1]FRED!CR337)*100</f>
+      <c r="AB336" s="9">
+        <v>-0.11441647597254005</v>
+      </c>
+      <c r="AC336" s="9">
+        <v>1.3086150490730675</v>
+      </c>
+      <c r="AD336" s="9">
+        <v>0.17452006980801799</v>
+      </c>
+      <c r="AE336" s="9">
+        <v>3.5272277227722881</v>
+      </c>
+      <c r="AF336" s="9">
+        <v>0.1111111111111048</v>
+      </c>
+      <c r="AG336" s="9">
+        <v>0.34190817323345962</v>
+      </c>
+      <c r="AH336" s="9">
+        <v>-0.37796976241900038</v>
+      </c>
+      <c r="AI336" s="9">
+        <v>8.9729431253447997E-2</v>
+      </c>
+      <c r="AJ336" s="9">
+        <v>0.77235772357724197</v>
+      </c>
+      <c r="AK336" s="9">
+        <v>-1.820388349514563</v>
+      </c>
+      <c r="AL336" s="9">
+        <v>0.42172523961660757</v>
+      </c>
+      <c r="AM336" s="9">
+        <v>0.51428571428571757</v>
+      </c>
+      <c r="AN336" s="9">
+        <v>-5.7244501940491554</v>
+      </c>
+      <c r="AO336" s="9">
+        <v>-0.87570621468927201</v>
+      </c>
+      <c r="AP336" s="9">
         <v>0</v>
       </c>
-      <c r="AW335" s="11">
-        <f>(([1]FRED!CP349-[1]FRED!CP337)/[1]FRED!CP337)*100</f>
-        <v>-0.76623014767344666</v>
-      </c>
-      <c r="AX335" s="11">
-        <f>(([1]FRED!CT349-[1]FRED!CT337)/[1]FRED!CT337)*100</f>
-        <v>0.97004765146356897</v>
-      </c>
-      <c r="AY335" s="11">
-        <f>(([1]FRED!CX349-[1]FRED!CX337)/[1]FRED!CX337)*100</f>
-        <v>0.58555627846454505</v>
-      </c>
-      <c r="AZ335" s="11">
-        <f>(([1]FRED!CV349-[1]FRED!CV337)/[1]FRED!CV337)*100</f>
-        <v>1.007618579503569</v>
-      </c>
-      <c r="BA335" s="11">
-        <f>(([1]FRED!CZ349-[1]FRED!CZ337)/[1]FRED!CZ337)*100</f>
-        <v>-2.1337126600284497</v>
-      </c>
-    </row>
-    <row r="336" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A336" s="7"/>
+      <c r="AQ336" s="9">
+        <v>-8.1455335324466846E-2</v>
+      </c>
+      <c r="AR336" s="9">
+        <v>0.37878787878787518</v>
+      </c>
+      <c r="AS336" s="9">
+        <v>6.9686411149828431E-2</v>
+      </c>
+      <c r="AT336" s="9">
+        <v>0.22697962342017491</v>
+      </c>
+      <c r="AU336" s="9">
+        <v>2.2643062988884313</v>
+      </c>
+      <c r="AV336" s="9">
+        <v>-0.35650623885918509</v>
+      </c>
+      <c r="AW336" s="9">
+        <v>-0.4043502509760305</v>
+      </c>
+      <c r="AX336" s="9">
+        <v>0.62669376693767709</v>
+      </c>
+      <c r="AY336" s="9">
+        <v>0.65019505851755521</v>
+      </c>
+      <c r="AZ336" s="9">
+        <v>7.3295870999269819E-2</v>
+      </c>
+      <c r="BA336" s="9">
+        <v>-0.99573257467994725</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A337" s="7"/>

</xml_diff>

<commit_message>
add december new stuff
</commit_message>
<xml_diff>
--- a/data/historical/source/gov_employment_historical.xlsx
+++ b/data/historical/source/gov_employment_historical.xlsx
@@ -183,7 +183,7 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Government Employment; Year/Year: January 1991 -- November 2018</t>
+    <t>Government Employment; Year/Year: January 1991 -- December 2018</t>
   </si>
 </sst>
 </file>
@@ -52149,7 +52149,7 @@
         <v>42736</v>
       </c>
       <c r="B318" s="8">
-        <v>0.90444534888979333</v>
+        <v>0.8635110086351101</v>
       </c>
       <c r="C318" s="8">
         <v>0.86659663865546521</v>
@@ -52310,7 +52310,7 @@
         <v>42767</v>
       </c>
       <c r="B319" s="8">
-        <v>0.77242750022585593</v>
+        <v>0.79024610521562422</v>
       </c>
       <c r="C319" s="8">
         <v>0.86659663865546521</v>
@@ -52471,7 +52471,7 @@
         <v>42795</v>
       </c>
       <c r="B320" s="8">
-        <v>0.63590853741036402</v>
+        <v>0.65816165532164272</v>
       </c>
       <c r="C320" s="8">
         <v>0.8923884514435636</v>
@@ -52632,7 +52632,7 @@
         <v>42826</v>
       </c>
       <c r="B321" s="8">
-        <v>0.62226631194480775</v>
+        <v>0.64446347289197348</v>
       </c>
       <c r="C321" s="8">
         <v>0.86546026750590388</v>
@@ -52793,7 +52793,7 @@
         <v>42856</v>
       </c>
       <c r="B322" s="8">
-        <v>0.5137217790996349</v>
+        <v>0.61722832942872596</v>
       </c>
       <c r="C322" s="8">
         <v>0.89145254326167644</v>
@@ -52954,7 +52954,7 @@
         <v>42887</v>
       </c>
       <c r="B323" s="9">
-        <v>0.61747870374543656</v>
+        <v>0.68909606809890556</v>
       </c>
       <c r="C323" s="9">
         <v>0.86387434554974118</v>
@@ -53115,7 +53115,7 @@
         <v>42917</v>
       </c>
       <c r="B324" s="9">
-        <v>0.20196580045778917</v>
+        <v>0.31392950040362366</v>
       </c>
       <c r="C324" s="9">
         <v>0.62679550796553518</v>
@@ -53276,7 +53276,7 @@
         <v>42948</v>
       </c>
       <c r="B325" s="9">
-        <v>0.24681385747621615</v>
+        <v>0.40411297202640206</v>
       </c>
       <c r="C325" s="9">
         <v>0.46887210210992741</v>
@@ -53437,7 +53437,7 @@
         <v>42979</v>
       </c>
       <c r="B326" s="9">
-        <v>0.12550988390335738</v>
+        <v>0.30050233225690709</v>
       </c>
       <c r="C326" s="9">
         <v>0.46936114732725198</v>
@@ -53598,7 +53598,7 @@
         <v>43009</v>
       </c>
       <c r="B327" s="9">
-        <v>0.13901345291479822</v>
+        <v>0.35884094375168207</v>
       </c>
       <c r="C327" s="9">
         <v>0.2607561929595828</v>
@@ -53759,7 +53759,7 @@
         <v>43040</v>
       </c>
       <c r="B328" s="9">
-        <v>0.14351062875594225</v>
+        <v>0.45780969479353684</v>
       </c>
       <c r="C328" s="9">
         <v>0.33898305084746061</v>
@@ -53920,7 +53920,7 @@
         <v>43070</v>
       </c>
       <c r="B329" s="9">
-        <v>0.11207746794584417</v>
+        <v>0.38109756097560976</v>
       </c>
       <c r="C329" s="9">
         <v>0.13024225058609012</v>
@@ -54081,7 +54081,7 @@
         <v>43101</v>
       </c>
       <c r="B330" s="9">
-        <v>2.6890153722045441E-2</v>
+        <v>0.2868668758404303</v>
       </c>
       <c r="C330" s="9">
         <v>0.10413954699296465</v>
@@ -54242,7 +54242,7 @@
         <v>43132</v>
       </c>
       <c r="B331" s="9">
-        <v>5.827244609798736E-2</v>
+        <v>0.35842293906810035</v>
       </c>
       <c r="C331" s="9">
         <v>0.31241864097890876</v>
@@ -54403,7 +54403,7 @@
         <v>43160</v>
       </c>
       <c r="B332" s="9">
-        <v>4.4814914403513491E-2</v>
+        <v>0.35827847194231716</v>
       </c>
       <c r="C332" s="9">
         <v>0.44224765868887761</v>
@@ -54564,7 +54564,7 @@
         <v>43191</v>
       </c>
       <c r="B333" s="9">
-        <v>4.4812906116961683E-2</v>
+        <v>0.39853125559734909</v>
       </c>
       <c r="C333" s="9">
         <v>0.4420176807072253</v>
@@ -54725,7 +54725,7 @@
         <v>43221</v>
       </c>
       <c r="B334" s="11">
-        <v>0.12553239184039452</v>
+        <v>0.42090180450454484</v>
       </c>
       <c r="C334" s="11">
         <v>0.23388773388772796</v>
@@ -54886,7 +54886,7 @@
         <v>43252</v>
       </c>
       <c r="B335" s="11">
-        <v>0.11198709908618526</v>
+        <v>0.43388799427446767</v>
       </c>
       <c r="C335" s="11">
         <v>-0.28549182455230282</v>
@@ -55047,7 +55047,7 @@
         <v>43282</v>
       </c>
       <c r="B336" s="9">
-        <v>0.22843321687718354</v>
+        <v>0.4023605150214592</v>
       </c>
       <c r="C336" s="9">
         <v>-0.33739942901635384</v>
@@ -55208,7 +55208,7 @@
         <v>43313</v>
       </c>
       <c r="B337" s="9">
-        <v>0.25515913872599494</v>
+        <v>0.59478556415187156</v>
       </c>
       <c r="C337" s="9">
         <v>-7.7780658542911954E-2</v>
@@ -55369,7 +55369,7 @@
         <v>43344</v>
       </c>
       <c r="B338" s="9">
-        <v>0.27308949276984373</v>
+        <v>0.5857890265170147</v>
       </c>
       <c r="C338" s="9">
         <v>0.57098364910459076</v>
@@ -55530,7 +55530,7 @@
         <v>43374</v>
       </c>
       <c r="B339" s="9">
-        <v>0.23733822936724733</v>
+        <v>0.50058103155448286</v>
       </c>
       <c r="C339" s="9">
         <v>0.54616384915475236</v>
@@ -55691,88 +55691,88 @@
         <v>43405</v>
       </c>
       <c r="B340" s="9">
-        <v>0.21495745633676669</v>
+        <v>0.4467875971763024</v>
       </c>
       <c r="C340" s="9">
-        <v>0.54573804573803686</v>
+        <v>0.72765072765073058</v>
       </c>
       <c r="D340" s="9">
         <v>-0.24752475247525105</v>
       </c>
       <c r="E340" s="9">
-        <v>1.11461109764963</v>
+        <v>0.96922704143445593</v>
       </c>
       <c r="F340" s="9">
-        <v>9.4607379375585915E-2</v>
+        <v>4.7303689687792957E-2</v>
       </c>
       <c r="G340" s="9">
-        <v>1.2234910277324633</v>
+        <v>1.2778684067427986</v>
       </c>
       <c r="H340" s="9">
-        <v>1.5692517625653934</v>
+        <v>1.5010234250625478</v>
       </c>
       <c r="I340" s="9">
-        <v>-1.427335640138401</v>
+        <v>-1.3840830449826942</v>
       </c>
       <c r="J340" s="9">
-        <v>1.0526315789473728</v>
+        <v>0.90225563909773576</v>
       </c>
       <c r="K340" s="9">
-        <v>-1.0878661087866086</v>
+        <v>-0.87866108786610642</v>
       </c>
       <c r="L340" s="9">
-        <v>-0.86548864046160612</v>
+        <v>-0.76631806707536965</v>
       </c>
       <c r="M340" s="9">
-        <v>0.34732272069464215</v>
+        <v>0.47756874095513091</v>
       </c>
       <c r="N340" s="9">
-        <v>2.9220779220779174</v>
+        <v>3.490259740259738</v>
       </c>
       <c r="O340" s="9">
         <v>1.6</v>
       </c>
       <c r="P340" s="9">
-        <v>1.7805582290664046</v>
+        <v>2.1655437921077958</v>
       </c>
       <c r="Q340" s="9">
-        <v>0.11734334663224594</v>
+        <v>0.16428068528514167</v>
       </c>
       <c r="R340" s="9">
-        <v>0.11556240369797939</v>
+        <v>3.8520801232652502E-2</v>
       </c>
       <c r="S340" s="9">
-        <v>1.0911925175370047</v>
+        <v>1.1301636788776217</v>
       </c>
       <c r="T340" s="9">
-        <v>-9.5268339155272955E-2</v>
+        <v>-0.15878056525881235</v>
       </c>
       <c r="U340" s="9">
         <v>-0.64377682403432435</v>
       </c>
       <c r="V340" s="9">
-        <v>0.19980019980020267</v>
+        <v>9.9900099900108424E-2</v>
       </c>
       <c r="W340" s="9">
-        <v>0.11916583912612169</v>
+        <v>-0.17874875868917126</v>
       </c>
       <c r="X340" s="9">
-        <v>-4.4228217602828093E-2</v>
+        <v>6.6342326404248433E-2</v>
       </c>
       <c r="Y340" s="9">
-        <v>0.70561207745324395</v>
+        <v>0.55792582868394769</v>
       </c>
       <c r="Z340" s="9">
-        <v>0.51401869158878233</v>
+        <v>0.44392523364485448</v>
       </c>
       <c r="AA340" s="9">
-        <v>0.82236842105263153</v>
+        <v>0.78125000000000244</v>
       </c>
       <c r="AB340" s="9">
-        <v>0.27726432532347239</v>
+        <v>0.3234750462107156</v>
       </c>
       <c r="AC340" s="9">
-        <v>0.76335877862595725</v>
+        <v>0.98146128680478895</v>
       </c>
       <c r="AD340" s="9">
         <v>0.29002320185614849</v>
@@ -55781,7 +55781,7 @@
         <v>2.7472527472527473</v>
       </c>
       <c r="AF340" s="9">
-        <v>1.1123470522803114</v>
+        <v>1.2235817575083363</v>
       </c>
       <c r="AG340" s="9">
         <v>-0.16252234682268815</v>
@@ -55790,13 +55790,13 @@
         <v>0.32085561497325898</v>
       </c>
       <c r="AI340" s="9">
-        <v>0.17260425296879314</v>
+        <v>0.17950842308753859</v>
       </c>
       <c r="AJ340" s="9">
-        <v>0.51735874744723676</v>
+        <v>0.54458815520762416</v>
       </c>
       <c r="AK340" s="9">
-        <v>-1.2239902080783354</v>
+        <v>-1.3463892288861794</v>
       </c>
       <c r="AL340" s="9">
         <v>1.0226255912054198</v>
@@ -55805,25 +55805,25 @@
         <v>0.22779043280182557</v>
       </c>
       <c r="AN340" s="9">
-        <v>-3.9805825242718482</v>
+        <v>-3.8511326860841346</v>
       </c>
       <c r="AO340" s="9">
-        <v>2.8518465706551473E-2</v>
+        <v>-8.5555397119621998E-2</v>
       </c>
       <c r="AP340" s="9">
         <v>-0.32840722495894209</v>
       </c>
       <c r="AQ340" s="9">
-        <v>0.90040927694406869</v>
+        <v>0.84583901773534043</v>
       </c>
       <c r="AR340" s="9">
-        <v>0.87719298245614397</v>
+        <v>0.75187969924813103</v>
       </c>
       <c r="AS340" s="9">
-        <v>0.37002775208141137</v>
+        <v>0.39315448658650448</v>
       </c>
       <c r="AT340" s="9">
-        <v>8.7592745259689075E-2</v>
+        <v>0.11850783182192676</v>
       </c>
       <c r="AU340" s="9">
         <v>2.2412387938060307</v>
@@ -55832,23 +55832,181 @@
         <v>0.17921146953405273</v>
       </c>
       <c r="AW340" s="9">
-        <v>-2.2476615943040499</v>
+        <v>-2.3872679045092711</v>
       </c>
       <c r="AX340" s="9">
-        <v>0.44060328757838041</v>
+        <v>0.83036773428232113</v>
       </c>
       <c r="AY340" s="9">
-        <v>1.041666666666663</v>
+        <v>1.1718750000000075</v>
       </c>
       <c r="AZ340" s="9">
-        <v>0.81521739130435056</v>
+        <v>1.2104743083003897</v>
       </c>
       <c r="BA340" s="9">
-        <v>-0.28776978417266597</v>
+        <v>-0.14388489208632277</v>
       </c>
     </row>
     <row r="341" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7">
+        <v>43435</v>
+      </c>
+      <c r="B341" s="9">
+        <v>0.48684621912546344</v>
+      </c>
+      <c r="C341" s="9">
+        <v>1.222684703433935</v>
+      </c>
+      <c r="D341" s="9">
+        <v>-0.24875621890547614</v>
+      </c>
+      <c r="E341" s="9">
+        <v>1.0419190695420431</v>
+      </c>
+      <c r="F341" s="9">
+        <v>4.7326076668241512E-2</v>
+      </c>
+      <c r="G341" s="9">
+        <v>1.1748284285215844</v>
+      </c>
+      <c r="H341" s="9">
+        <v>1.5909090909090908</v>
+      </c>
+      <c r="I341" s="9">
+        <v>-1.5577672003461682</v>
+      </c>
+      <c r="J341" s="9">
+        <v>1.2048192771084292</v>
+      </c>
+      <c r="K341" s="9">
+        <v>-0.62893081761006298</v>
+      </c>
+      <c r="L341" s="9">
+        <v>-0.88177073960771823</v>
+      </c>
+      <c r="M341" s="9">
+        <v>1.0635198135198234</v>
+      </c>
+      <c r="N341" s="9">
+        <v>0.47808764940238591</v>
+      </c>
+      <c r="O341" s="9">
+        <v>2.1582733812949666</v>
+      </c>
+      <c r="P341" s="9">
+        <v>2.9730380356283157</v>
+      </c>
+      <c r="Q341" s="9">
+        <v>0.42253521126760829</v>
+      </c>
+      <c r="R341" s="9">
+        <v>0.42438271604939154</v>
+      </c>
+      <c r="S341" s="9">
+        <v>1.1292834890965644</v>
+      </c>
+      <c r="T341" s="9">
+        <v>-0.22250476795932783</v>
+      </c>
+      <c r="U341" s="9">
+        <v>-0.583538083538094</v>
+      </c>
+      <c r="V341" s="9">
+        <v>0.20040080160320925</v>
+      </c>
+      <c r="W341" s="9">
+        <v>-1.9864918553827157E-2</v>
+      </c>
+      <c r="X341" s="9">
+        <v>-4.4169611307417984E-2</v>
+      </c>
+      <c r="Y341" s="9">
+        <v>0.36065573770492548</v>
+      </c>
+      <c r="Z341" s="9">
+        <v>0.65573770491803551</v>
+      </c>
+      <c r="AA341" s="9">
+        <v>0.57589469354175471</v>
+      </c>
+      <c r="AB341" s="9">
+        <v>0.50890585241730013</v>
+      </c>
+      <c r="AC341" s="9">
+        <v>1.3086150490730675</v>
+      </c>
+      <c r="AD341" s="9">
+        <v>0.69767441860464452</v>
+      </c>
+      <c r="AE341" s="9">
+        <v>3.3700980392156867</v>
+      </c>
+      <c r="AF341" s="9">
+        <v>1.336302895322943</v>
+      </c>
+      <c r="AG341" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH341" s="9">
+        <v>0.42735042735043349</v>
+      </c>
+      <c r="AI341" s="9">
+        <v>0.14491753502174706</v>
+      </c>
+      <c r="AJ341" s="9">
+        <v>0.61266167460857723</v>
+      </c>
+      <c r="AK341" s="9">
+        <v>-0.73529411764705188</v>
+      </c>
+      <c r="AL341" s="9">
+        <v>1.496163682864456</v>
+      </c>
+      <c r="AM341" s="9">
+        <v>0.34188034188033861</v>
+      </c>
+      <c r="AN341" s="9">
+        <v>-3.8399483704420709</v>
+      </c>
+      <c r="AO341" s="9">
+        <v>0.30012862655422451</v>
+      </c>
+      <c r="AP341" s="9">
+        <v>-0.16420361247947687</v>
+      </c>
+      <c r="AQ341" s="9">
+        <v>0.81788440567066523</v>
+      </c>
+      <c r="AR341" s="9">
+        <v>0.7528230865746478</v>
+      </c>
+      <c r="AS341" s="9">
+        <v>0.74263170109075094</v>
+      </c>
+      <c r="AT341" s="9">
+        <v>0.1544242549029701</v>
+      </c>
+      <c r="AU341" s="9">
+        <v>2.2792022792022886</v>
+      </c>
+      <c r="AV341" s="9">
+        <v>-0.1788908765652977</v>
+      </c>
+      <c r="AW341" s="9">
+        <v>-2.2203602848764108</v>
+      </c>
+      <c r="AX341" s="9">
+        <v>0.99881496529540836</v>
+      </c>
+      <c r="AY341" s="9">
+        <v>1.3671874999999964</v>
+      </c>
+      <c r="AZ341" s="9">
+        <v>0.83682008368200278</v>
+      </c>
+      <c r="BA341" s="9">
+        <v>-0.14409221902018518</v>
+      </c>
     </row>
     <row r="342" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A342" s="7"/>

</xml_diff>